<commit_message>
Get cats by id
</commit_message>
<xml_diff>
--- a/DataBase/BreedCatsData.xlsx
+++ b/DataBase/BreedCatsData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\source\repos\CatsCenter\DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97240BB0-6779-4C1B-BA99-4D29A166F7EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EFB6C0-2B81-4A70-A742-B32058606A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18045" yWindow="3960" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{F0E8892A-E61F-468D-BA28-553DFEA2DB6C}"/>
+    <workbookView xWindow="26160" yWindow="5490" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{F0E8892A-E61F-468D-BA28-553DFEA2DB6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="462">
   <si>
     <r>
       <t>Abyssinian</t>
@@ -3444,6 +3444,168 @@
   </si>
   <si>
     <t>Orange</t>
+  </si>
+  <si>
+    <t>Leopard</t>
+  </si>
+  <si>
+    <t>Lion</t>
+  </si>
+  <si>
+    <t>Jaguar</t>
+  </si>
+  <si>
+    <t>Snow leopard</t>
+  </si>
+  <si>
+    <t>Tiger</t>
+  </si>
+  <si>
+    <t>Clouded leopard</t>
+  </si>
+  <si>
+    <t>Caracal</t>
+  </si>
+  <si>
+    <t>African golden cat</t>
+  </si>
+  <si>
+    <t>Serval</t>
+  </si>
+  <si>
+    <t>Geoffroy's cat</t>
+  </si>
+  <si>
+    <t>Kodkod</t>
+  </si>
+  <si>
+    <t>Southern tiger cat</t>
+  </si>
+  <si>
+    <t>Oncilla</t>
+  </si>
+  <si>
+    <t>Pampas cat</t>
+  </si>
+  <si>
+    <t>Andean mountain cat</t>
+  </si>
+  <si>
+    <t>Ocelot</t>
+  </si>
+  <si>
+    <t>Margay</t>
+  </si>
+  <si>
+    <t>Bay cat</t>
+  </si>
+  <si>
+    <t>Asian golden cat</t>
+  </si>
+  <si>
+    <t>Marbled cat</t>
+  </si>
+  <si>
+    <t>Eurasian lynx</t>
+  </si>
+  <si>
+    <t>Iberian lynx</t>
+  </si>
+  <si>
+    <t>Canada lynx</t>
+  </si>
+  <si>
+    <t>Bobcat</t>
+  </si>
+  <si>
+    <t>Puma</t>
+  </si>
+  <si>
+    <t>Jaguarundi</t>
+  </si>
+  <si>
+    <t>Cheetah</t>
+  </si>
+  <si>
+    <t>Sunda leopard cat</t>
+  </si>
+  <si>
+    <t>Leopard cat</t>
+  </si>
+  <si>
+    <t>Fishing cat</t>
+  </si>
+  <si>
+    <t>Flat-headed cat</t>
+  </si>
+  <si>
+    <t>Rusty-spotted cat</t>
+  </si>
+  <si>
+    <t>Pallas's cat</t>
+  </si>
+  <si>
+    <t>Jungle cat</t>
+  </si>
+  <si>
+    <t>Black-footed cat</t>
+  </si>
+  <si>
+    <t>Sand cat</t>
+  </si>
+  <si>
+    <t>Chineese mountain cat</t>
+  </si>
+  <si>
+    <t>African wildcat</t>
+  </si>
+  <si>
+    <t>European wildcat</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Slender</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Yellow-gold</t>
+  </si>
+  <si>
+    <t>Black spots</t>
+  </si>
+  <si>
+    <t>Tanwy</t>
+  </si>
+  <si>
+    <t>Yellow-orange</t>
+  </si>
+  <si>
+    <t>Grayish-white</t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>Black stripes</t>
+  </si>
+  <si>
+    <t>Black cloud patterns</t>
+  </si>
+  <si>
+    <t>Reddish brown</t>
+  </si>
+  <si>
+    <t>Golden</t>
+  </si>
+  <si>
+    <t>Grayish</t>
   </si>
 </sst>
 </file>
@@ -3686,6 +3848,28 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3704,24 +3888,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3731,10 +3897,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -10070,66 +10232,66 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="29" t="s">
         <v>39</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="F13" s="26" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="8"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="8"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="9"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
     </row>
     <row r="18" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
     </row>
     <row r="19" spans="1:6" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
@@ -10152,120 +10314,120 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="29" t="s">
         <v>50</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="D20" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="26" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="8"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="9"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
     </row>
     <row r="23" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23"/>
+      <c r="A23" s="31"/>
       <c r="B23" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
     </row>
     <row r="24" spans="1:6" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="29" t="s">
         <v>56</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="27" t="s">
+      <c r="F24" s="26" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="8"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="8"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="8"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="8"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="9"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
     </row>
     <row r="30" spans="1:6" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="23"/>
+      <c r="A30" s="31"/>
       <c r="B30" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
     </row>
     <row r="31" spans="1:6" ht="143.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
@@ -10488,66 +10650,66 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="29" t="s">
         <v>95</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C42" s="27" t="s">
+      <c r="C42" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D42" s="27" t="s">
+      <c r="D42" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E42" s="27" t="s">
+      <c r="E42" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="F42" s="27" t="s">
+      <c r="F42" s="26" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
+      <c r="A43" s="30"/>
       <c r="B43" s="8"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
+      <c r="A44" s="30"/>
       <c r="B44" s="8"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
+      <c r="A45" s="30"/>
       <c r="B45" s="8"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="27"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="8"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="28"/>
-      <c r="F46" s="28"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="27"/>
     </row>
     <row r="47" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="23"/>
+      <c r="A47" s="31"/>
       <c r="B47" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
     </row>
     <row r="48" spans="1:6" ht="111.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
@@ -10613,117 +10775,117 @@
       <c r="A51" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B51" s="27" t="s">
+      <c r="B51" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="C51" s="27" t="s">
+      <c r="C51" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D51" s="27" t="s">
+      <c r="D51" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E51" s="27" t="s">
+      <c r="E51" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="F51" s="27" t="s">
+      <c r="F51" s="26" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
-      <c r="B52" s="28"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="28"/>
-      <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="27"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
-      <c r="B53" s="28"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="27"/>
+      <c r="F53" s="27"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="14"/>
-      <c r="B54" s="28"/>
-      <c r="C54" s="28"/>
-      <c r="D54" s="28"/>
-      <c r="E54" s="28"/>
-      <c r="F54" s="28"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="27"/>
+      <c r="F54" s="27"/>
     </row>
     <row r="55" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B55" s="29"/>
-      <c r="C55" s="29"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="29"/>
-      <c r="F55" s="29"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="28"/>
     </row>
     <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B56" s="27" t="s">
+      <c r="B56" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="C56" s="27" t="s">
+      <c r="C56" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D56" s="27" t="s">
+      <c r="D56" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="E56" s="27" t="s">
+      <c r="E56" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F56" s="27" t="s">
+      <c r="F56" s="26" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="13"/>
-      <c r="B57" s="28"/>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="28"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
-      <c r="B58" s="28"/>
-      <c r="C58" s="28"/>
-      <c r="D58" s="28"/>
-      <c r="E58" s="28"/>
-      <c r="F58" s="28"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="27"/>
+      <c r="F58" s="27"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
-      <c r="B59" s="28"/>
-      <c r="C59" s="28"/>
-      <c r="D59" s="28"/>
-      <c r="E59" s="28"/>
-      <c r="F59" s="28"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="27"/>
+      <c r="F59" s="27"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="14"/>
-      <c r="B60" s="28"/>
-      <c r="C60" s="28"/>
-      <c r="D60" s="28"/>
-      <c r="E60" s="28"/>
-      <c r="F60" s="28"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="27"/>
+      <c r="F60" s="27"/>
     </row>
     <row r="61" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B61" s="29"/>
-      <c r="C61" s="29"/>
-      <c r="D61" s="29"/>
-      <c r="E61" s="29"/>
-      <c r="F61" s="29"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="28"/>
+      <c r="F61" s="28"/>
     </row>
     <row r="62" spans="1:6" ht="129" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
@@ -10846,58 +11008,58 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="85.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="21" t="s">
+      <c r="A68" s="29" t="s">
         <v>123</v>
       </c>
       <c r="B68" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="C68" s="27" t="s">
+      <c r="C68" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="D68" s="27" t="s">
+      <c r="D68" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E68" s="27" t="s">
+      <c r="E68" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F68" s="27" t="s">
+      <c r="F68" s="26" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="22"/>
+      <c r="A69" s="30"/>
       <c r="B69" s="8"/>
-      <c r="C69" s="28"/>
-      <c r="D69" s="28"/>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
+      <c r="C69" s="27"/>
+      <c r="D69" s="27"/>
+      <c r="E69" s="27"/>
+      <c r="F69" s="27"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="22"/>
+      <c r="A70" s="30"/>
       <c r="B70" s="8"/>
-      <c r="C70" s="28"/>
-      <c r="D70" s="28"/>
-      <c r="E70" s="28"/>
-      <c r="F70" s="28"/>
+      <c r="C70" s="27"/>
+      <c r="D70" s="27"/>
+      <c r="E70" s="27"/>
+      <c r="F70" s="27"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="22"/>
+      <c r="A71" s="30"/>
       <c r="B71" s="9"/>
-      <c r="C71" s="28"/>
-      <c r="D71" s="28"/>
-      <c r="E71" s="28"/>
-      <c r="F71" s="28"/>
+      <c r="C71" s="27"/>
+      <c r="D71" s="27"/>
+      <c r="E71" s="27"/>
+      <c r="F71" s="27"/>
     </row>
     <row r="72" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="23"/>
+      <c r="A72" s="31"/>
       <c r="B72" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C72" s="29"/>
-      <c r="D72" s="29"/>
-      <c r="E72" s="29"/>
-      <c r="F72" s="29"/>
+      <c r="C72" s="28"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="28"/>
+      <c r="F72" s="28"/>
     </row>
     <row r="73" spans="1:6" ht="114.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
@@ -10923,55 +11085,55 @@
       <c r="A74" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B74" s="24" t="s">
+      <c r="B74" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="C74" s="27" t="s">
+      <c r="C74" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="D74" s="27" t="s">
+      <c r="D74" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E74" s="27" t="s">
+      <c r="E74" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="F74" s="27" t="s">
+      <c r="F74" s="26" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="13"/>
-      <c r="B75" s="25"/>
-      <c r="C75" s="28"/>
-      <c r="D75" s="28"/>
-      <c r="E75" s="28"/>
-      <c r="F75" s="28"/>
+      <c r="B75" s="33"/>
+      <c r="C75" s="27"/>
+      <c r="D75" s="27"/>
+      <c r="E75" s="27"/>
+      <c r="F75" s="27"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="13"/>
-      <c r="B76" s="25"/>
-      <c r="C76" s="28"/>
-      <c r="D76" s="28"/>
-      <c r="E76" s="28"/>
-      <c r="F76" s="28"/>
+      <c r="B76" s="33"/>
+      <c r="C76" s="27"/>
+      <c r="D76" s="27"/>
+      <c r="E76" s="27"/>
+      <c r="F76" s="27"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="14"/>
-      <c r="B77" s="25"/>
-      <c r="C77" s="28"/>
-      <c r="D77" s="28"/>
-      <c r="E77" s="28"/>
-      <c r="F77" s="28"/>
+      <c r="B77" s="33"/>
+      <c r="C77" s="27"/>
+      <c r="D77" s="27"/>
+      <c r="E77" s="27"/>
+      <c r="F77" s="27"/>
     </row>
     <row r="78" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="B78" s="26"/>
-      <c r="C78" s="29"/>
-      <c r="D78" s="29"/>
-      <c r="E78" s="29"/>
-      <c r="F78" s="29"/>
+      <c r="B78" s="34"/>
+      <c r="C78" s="28"/>
+      <c r="D78" s="28"/>
+      <c r="E78" s="28"/>
+      <c r="F78" s="28"/>
     </row>
     <row r="79" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
@@ -11000,16 +11162,16 @@
       <c r="B80" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C80" s="27" t="s">
+      <c r="C80" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="D80" s="27" t="s">
+      <c r="D80" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="E80" s="27" t="s">
+      <c r="E80" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="F80" s="27" t="s">
+      <c r="F80" s="26" t="s">
         <v>44</v>
       </c>
     </row>
@@ -11018,28 +11180,28 @@
       <c r="B81" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C81" s="28"/>
-      <c r="D81" s="28"/>
-      <c r="E81" s="28"/>
-      <c r="F81" s="28"/>
+      <c r="C81" s="27"/>
+      <c r="D81" s="27"/>
+      <c r="E81" s="27"/>
+      <c r="F81" s="27"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="14"/>
       <c r="B82" s="9"/>
-      <c r="C82" s="28"/>
-      <c r="D82" s="28"/>
-      <c r="E82" s="28"/>
-      <c r="F82" s="28"/>
+      <c r="C82" s="27"/>
+      <c r="D82" s="27"/>
+      <c r="E82" s="27"/>
+      <c r="F82" s="27"/>
     </row>
     <row r="83" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="16" t="s">
         <v>137</v>
       </c>
       <c r="B83" s="10"/>
-      <c r="C83" s="29"/>
-      <c r="D83" s="29"/>
-      <c r="E83" s="29"/>
-      <c r="F83" s="29"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="28"/>
+      <c r="E83" s="28"/>
+      <c r="F83" s="28"/>
     </row>
     <row r="84" spans="1:6" ht="143.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
@@ -11165,55 +11327,55 @@
       <c r="A90" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="B90" s="30" t="s">
+      <c r="B90" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="C90" s="27" t="s">
+      <c r="C90" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="D90" s="27" t="s">
+      <c r="D90" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="E90" s="24" t="s">
+      <c r="E90" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="F90" s="27" t="s">
+      <c r="F90" s="26" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="13"/>
-      <c r="B91" s="31"/>
-      <c r="C91" s="28"/>
-      <c r="D91" s="28"/>
-      <c r="E91" s="25"/>
-      <c r="F91" s="28"/>
+      <c r="B91" s="24"/>
+      <c r="C91" s="27"/>
+      <c r="D91" s="27"/>
+      <c r="E91" s="33"/>
+      <c r="F91" s="27"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="13"/>
-      <c r="B92" s="31"/>
-      <c r="C92" s="28"/>
-      <c r="D92" s="28"/>
-      <c r="E92" s="25"/>
-      <c r="F92" s="28"/>
+      <c r="B92" s="24"/>
+      <c r="C92" s="27"/>
+      <c r="D92" s="27"/>
+      <c r="E92" s="33"/>
+      <c r="F92" s="27"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="14"/>
-      <c r="B93" s="31"/>
-      <c r="C93" s="28"/>
-      <c r="D93" s="28"/>
-      <c r="E93" s="25"/>
-      <c r="F93" s="28"/>
+      <c r="B93" s="24"/>
+      <c r="C93" s="27"/>
+      <c r="D93" s="27"/>
+      <c r="E93" s="33"/>
+      <c r="F93" s="27"/>
     </row>
     <row r="94" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="B94" s="32"/>
-      <c r="C94" s="29"/>
-      <c r="D94" s="29"/>
-      <c r="E94" s="26"/>
-      <c r="F94" s="29"/>
+      <c r="B94" s="25"/>
+      <c r="C94" s="28"/>
+      <c r="D94" s="28"/>
+      <c r="E94" s="34"/>
+      <c r="F94" s="28"/>
     </row>
     <row r="95" spans="1:6" ht="114.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
@@ -11316,50 +11478,50 @@
       </c>
     </row>
     <row r="100" spans="1:6" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="21" t="s">
+      <c r="A100" s="29" t="s">
         <v>177</v>
       </c>
       <c r="B100" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="C100" s="27" t="s">
+      <c r="C100" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D100" s="27" t="s">
+      <c r="D100" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E100" s="27" t="s">
+      <c r="E100" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F100" s="27" t="s">
+      <c r="F100" s="26" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="22"/>
+      <c r="A101" s="30"/>
       <c r="B101" s="8"/>
-      <c r="C101" s="28"/>
-      <c r="D101" s="28"/>
-      <c r="E101" s="28"/>
-      <c r="F101" s="28"/>
+      <c r="C101" s="27"/>
+      <c r="D101" s="27"/>
+      <c r="E101" s="27"/>
+      <c r="F101" s="27"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="22"/>
+      <c r="A102" s="30"/>
       <c r="B102" s="9"/>
-      <c r="C102" s="28"/>
-      <c r="D102" s="28"/>
-      <c r="E102" s="28"/>
-      <c r="F102" s="28"/>
+      <c r="C102" s="27"/>
+      <c r="D102" s="27"/>
+      <c r="E102" s="27"/>
+      <c r="F102" s="27"/>
     </row>
     <row r="103" spans="1:6" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="23"/>
+      <c r="A103" s="31"/>
       <c r="B103" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C103" s="29"/>
-      <c r="D103" s="29"/>
-      <c r="E103" s="29"/>
-      <c r="F103" s="29"/>
+      <c r="C103" s="28"/>
+      <c r="D103" s="28"/>
+      <c r="E103" s="28"/>
+      <c r="F103" s="28"/>
     </row>
     <row r="104" spans="1:6" ht="143.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
@@ -11525,347 +11687,347 @@
       <c r="A112" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="B112" s="27" t="s">
+      <c r="B112" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="C112" s="27" t="s">
+      <c r="C112" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D112" s="27"/>
-      <c r="E112" s="27" t="s">
+      <c r="D112" s="26"/>
+      <c r="E112" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="F112" s="27"/>
+      <c r="F112" s="26"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="13"/>
-      <c r="B113" s="28"/>
-      <c r="C113" s="28"/>
-      <c r="D113" s="28"/>
-      <c r="E113" s="28"/>
-      <c r="F113" s="28"/>
+      <c r="B113" s="27"/>
+      <c r="C113" s="27"/>
+      <c r="D113" s="27"/>
+      <c r="E113" s="27"/>
+      <c r="F113" s="27"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="13"/>
-      <c r="B114" s="28"/>
-      <c r="C114" s="28"/>
-      <c r="D114" s="28"/>
-      <c r="E114" s="28"/>
-      <c r="F114" s="28"/>
+      <c r="B114" s="27"/>
+      <c r="C114" s="27"/>
+      <c r="D114" s="27"/>
+      <c r="E114" s="27"/>
+      <c r="F114" s="27"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="13"/>
-      <c r="B115" s="28"/>
-      <c r="C115" s="28"/>
-      <c r="D115" s="28"/>
-      <c r="E115" s="28"/>
-      <c r="F115" s="28"/>
+      <c r="B115" s="27"/>
+      <c r="C115" s="27"/>
+      <c r="D115" s="27"/>
+      <c r="E115" s="27"/>
+      <c r="F115" s="27"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="13"/>
-      <c r="B116" s="28"/>
-      <c r="C116" s="28"/>
-      <c r="D116" s="28"/>
-      <c r="E116" s="28"/>
-      <c r="F116" s="28"/>
+      <c r="B116" s="27"/>
+      <c r="C116" s="27"/>
+      <c r="D116" s="27"/>
+      <c r="E116" s="27"/>
+      <c r="F116" s="27"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="13"/>
-      <c r="B117" s="28"/>
-      <c r="C117" s="28"/>
-      <c r="D117" s="28"/>
-      <c r="E117" s="28"/>
-      <c r="F117" s="28"/>
+      <c r="B117" s="27"/>
+      <c r="C117" s="27"/>
+      <c r="D117" s="27"/>
+      <c r="E117" s="27"/>
+      <c r="F117" s="27"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="18"/>
-      <c r="B118" s="28"/>
-      <c r="C118" s="28"/>
-      <c r="D118" s="28"/>
-      <c r="E118" s="28"/>
-      <c r="F118" s="28"/>
+      <c r="B118" s="27"/>
+      <c r="C118" s="27"/>
+      <c r="D118" s="27"/>
+      <c r="E118" s="27"/>
+      <c r="F118" s="27"/>
     </row>
     <row r="119" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="B119" s="29"/>
-      <c r="C119" s="29"/>
-      <c r="D119" s="29"/>
-      <c r="E119" s="29"/>
-      <c r="F119" s="29"/>
+      <c r="B119" s="28"/>
+      <c r="C119" s="28"/>
+      <c r="D119" s="28"/>
+      <c r="E119" s="28"/>
+      <c r="F119" s="28"/>
     </row>
     <row r="120" spans="1:6" ht="171" x14ac:dyDescent="0.25">
-      <c r="A120" s="21" t="s">
+      <c r="A120" s="29" t="s">
         <v>202</v>
       </c>
       <c r="B120" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="C120" s="27" t="s">
+      <c r="C120" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="D120" s="27" t="s">
+      <c r="D120" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="E120" s="27" t="s">
+      <c r="E120" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F120" s="27" t="s">
+      <c r="F120" s="26" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="23"/>
+      <c r="A121" s="31"/>
       <c r="B121" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="C121" s="29"/>
-      <c r="D121" s="29"/>
-      <c r="E121" s="29"/>
-      <c r="F121" s="29"/>
+      <c r="C121" s="28"/>
+      <c r="D121" s="28"/>
+      <c r="E121" s="28"/>
+      <c r="F121" s="28"/>
     </row>
     <row r="122" spans="1:6" ht="114" x14ac:dyDescent="0.25">
-      <c r="A122" s="33" t="s">
+      <c r="A122" s="35" t="s">
         <v>207</v>
       </c>
       <c r="B122" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="C122" s="27" t="s">
+      <c r="C122" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="D122" s="27" t="s">
+      <c r="D122" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="E122" s="27" t="s">
+      <c r="E122" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F122" s="24" t="s">
+      <c r="F122" s="32" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="34"/>
+      <c r="A123" s="36"/>
       <c r="B123" s="8"/>
-      <c r="C123" s="28"/>
-      <c r="D123" s="28"/>
-      <c r="E123" s="28"/>
-      <c r="F123" s="25"/>
+      <c r="C123" s="27"/>
+      <c r="D123" s="27"/>
+      <c r="E123" s="27"/>
+      <c r="F123" s="33"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="34"/>
+      <c r="A124" s="36"/>
       <c r="B124" s="8"/>
-      <c r="C124" s="28"/>
-      <c r="D124" s="28"/>
-      <c r="E124" s="28"/>
-      <c r="F124" s="25"/>
+      <c r="C124" s="27"/>
+      <c r="D124" s="27"/>
+      <c r="E124" s="27"/>
+      <c r="F124" s="33"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="34"/>
+      <c r="A125" s="36"/>
       <c r="B125" s="8"/>
-      <c r="C125" s="28"/>
-      <c r="D125" s="28"/>
-      <c r="E125" s="28"/>
-      <c r="F125" s="25"/>
+      <c r="C125" s="27"/>
+      <c r="D125" s="27"/>
+      <c r="E125" s="27"/>
+      <c r="F125" s="33"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="34"/>
+      <c r="A126" s="36"/>
       <c r="B126" s="8"/>
-      <c r="C126" s="28"/>
-      <c r="D126" s="28"/>
-      <c r="E126" s="28"/>
-      <c r="F126" s="25"/>
+      <c r="C126" s="27"/>
+      <c r="D126" s="27"/>
+      <c r="E126" s="27"/>
+      <c r="F126" s="33"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="34"/>
+      <c r="A127" s="36"/>
       <c r="B127" s="8"/>
-      <c r="C127" s="28"/>
-      <c r="D127" s="28"/>
-      <c r="E127" s="28"/>
-      <c r="F127" s="25"/>
+      <c r="C127" s="27"/>
+      <c r="D127" s="27"/>
+      <c r="E127" s="27"/>
+      <c r="F127" s="33"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="34"/>
+      <c r="A128" s="36"/>
       <c r="B128" s="8"/>
-      <c r="C128" s="28"/>
-      <c r="D128" s="28"/>
-      <c r="E128" s="28"/>
-      <c r="F128" s="25"/>
+      <c r="C128" s="27"/>
+      <c r="D128" s="27"/>
+      <c r="E128" s="27"/>
+      <c r="F128" s="33"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="34"/>
+      <c r="A129" s="36"/>
       <c r="B129" s="9"/>
-      <c r="C129" s="28"/>
-      <c r="D129" s="28"/>
-      <c r="E129" s="28"/>
-      <c r="F129" s="25"/>
+      <c r="C129" s="27"/>
+      <c r="D129" s="27"/>
+      <c r="E129" s="27"/>
+      <c r="F129" s="33"/>
     </row>
     <row r="130" spans="1:6" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="35"/>
+      <c r="A130" s="37"/>
       <c r="B130" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="C130" s="29"/>
-      <c r="D130" s="29"/>
-      <c r="E130" s="29"/>
-      <c r="F130" s="26"/>
+      <c r="C130" s="28"/>
+      <c r="D130" s="28"/>
+      <c r="E130" s="28"/>
+      <c r="F130" s="34"/>
     </row>
     <row r="131" spans="1:6" ht="114" x14ac:dyDescent="0.25">
-      <c r="A131" s="33" t="s">
+      <c r="A131" s="35" t="s">
         <v>212</v>
       </c>
       <c r="B131" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="C131" s="27" t="s">
+      <c r="C131" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="D131" s="27" t="s">
+      <c r="D131" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="E131" s="27" t="s">
+      <c r="E131" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F131" s="27" t="s">
+      <c r="F131" s="26" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A132" s="34"/>
+      <c r="A132" s="36"/>
       <c r="B132" s="8"/>
-      <c r="C132" s="28"/>
-      <c r="D132" s="28"/>
-      <c r="E132" s="28"/>
-      <c r="F132" s="28"/>
+      <c r="C132" s="27"/>
+      <c r="D132" s="27"/>
+      <c r="E132" s="27"/>
+      <c r="F132" s="27"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A133" s="34"/>
+      <c r="A133" s="36"/>
       <c r="B133" s="8"/>
-      <c r="C133" s="28"/>
-      <c r="D133" s="28"/>
-      <c r="E133" s="28"/>
-      <c r="F133" s="28"/>
+      <c r="C133" s="27"/>
+      <c r="D133" s="27"/>
+      <c r="E133" s="27"/>
+      <c r="F133" s="27"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" s="34"/>
+      <c r="A134" s="36"/>
       <c r="B134" s="8"/>
-      <c r="C134" s="28"/>
-      <c r="D134" s="28"/>
-      <c r="E134" s="28"/>
-      <c r="F134" s="28"/>
+      <c r="C134" s="27"/>
+      <c r="D134" s="27"/>
+      <c r="E134" s="27"/>
+      <c r="F134" s="27"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="34"/>
+      <c r="A135" s="36"/>
       <c r="B135" s="8"/>
-      <c r="C135" s="28"/>
-      <c r="D135" s="28"/>
-      <c r="E135" s="28"/>
-      <c r="F135" s="28"/>
+      <c r="C135" s="27"/>
+      <c r="D135" s="27"/>
+      <c r="E135" s="27"/>
+      <c r="F135" s="27"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="34"/>
+      <c r="A136" s="36"/>
       <c r="B136" s="8"/>
-      <c r="C136" s="28"/>
-      <c r="D136" s="28"/>
-      <c r="E136" s="28"/>
-      <c r="F136" s="28"/>
+      <c r="C136" s="27"/>
+      <c r="D136" s="27"/>
+      <c r="E136" s="27"/>
+      <c r="F136" s="27"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" s="34"/>
+      <c r="A137" s="36"/>
       <c r="B137" s="8"/>
-      <c r="C137" s="28"/>
-      <c r="D137" s="28"/>
-      <c r="E137" s="28"/>
-      <c r="F137" s="28"/>
+      <c r="C137" s="27"/>
+      <c r="D137" s="27"/>
+      <c r="E137" s="27"/>
+      <c r="F137" s="27"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138" s="34"/>
+      <c r="A138" s="36"/>
       <c r="B138" s="8"/>
-      <c r="C138" s="28"/>
-      <c r="D138" s="28"/>
-      <c r="E138" s="28"/>
-      <c r="F138" s="28"/>
+      <c r="C138" s="27"/>
+      <c r="D138" s="27"/>
+      <c r="E138" s="27"/>
+      <c r="F138" s="27"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A139" s="34"/>
+      <c r="A139" s="36"/>
       <c r="B139" s="8"/>
-      <c r="C139" s="28"/>
-      <c r="D139" s="28"/>
-      <c r="E139" s="28"/>
-      <c r="F139" s="28"/>
+      <c r="C139" s="27"/>
+      <c r="D139" s="27"/>
+      <c r="E139" s="27"/>
+      <c r="F139" s="27"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A140" s="34"/>
+      <c r="A140" s="36"/>
       <c r="B140" s="9"/>
-      <c r="C140" s="28"/>
-      <c r="D140" s="28"/>
-      <c r="E140" s="28"/>
-      <c r="F140" s="28"/>
+      <c r="C140" s="27"/>
+      <c r="D140" s="27"/>
+      <c r="E140" s="27"/>
+      <c r="F140" s="27"/>
     </row>
     <row r="141" spans="1:6" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="35"/>
+      <c r="A141" s="37"/>
       <c r="B141" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="C141" s="29"/>
-      <c r="D141" s="29"/>
-      <c r="E141" s="29"/>
-      <c r="F141" s="29"/>
+      <c r="C141" s="28"/>
+      <c r="D141" s="28"/>
+      <c r="E141" s="28"/>
+      <c r="F141" s="28"/>
     </row>
     <row r="142" spans="1:6" ht="85.5" x14ac:dyDescent="0.25">
-      <c r="A142" s="21" t="s">
+      <c r="A142" s="29" t="s">
         <v>214</v>
       </c>
       <c r="B142" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="C142" s="27" t="s">
+      <c r="C142" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="D142" s="27" t="s">
+      <c r="D142" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E142" s="27" t="s">
+      <c r="E142" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="F142" s="27" t="s">
+      <c r="F142" s="26" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A143" s="22"/>
+      <c r="A143" s="30"/>
       <c r="B143" s="8"/>
-      <c r="C143" s="28"/>
-      <c r="D143" s="28"/>
-      <c r="E143" s="28"/>
-      <c r="F143" s="28"/>
+      <c r="C143" s="27"/>
+      <c r="D143" s="27"/>
+      <c r="E143" s="27"/>
+      <c r="F143" s="27"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A144" s="22"/>
+      <c r="A144" s="30"/>
       <c r="B144" s="8"/>
-      <c r="C144" s="28"/>
-      <c r="D144" s="28"/>
-      <c r="E144" s="28"/>
-      <c r="F144" s="28"/>
+      <c r="C144" s="27"/>
+      <c r="D144" s="27"/>
+      <c r="E144" s="27"/>
+      <c r="F144" s="27"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A145" s="22"/>
+      <c r="A145" s="30"/>
       <c r="B145" s="9"/>
-      <c r="C145" s="28"/>
-      <c r="D145" s="28"/>
-      <c r="E145" s="28"/>
-      <c r="F145" s="28"/>
+      <c r="C145" s="27"/>
+      <c r="D145" s="27"/>
+      <c r="E145" s="27"/>
+      <c r="F145" s="27"/>
     </row>
     <row r="146" spans="1:6" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="23"/>
+      <c r="A146" s="31"/>
       <c r="B146" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="C146" s="29"/>
-      <c r="D146" s="29"/>
-      <c r="E146" s="29"/>
-      <c r="F146" s="29"/>
+      <c r="C146" s="28"/>
+      <c r="D146" s="28"/>
+      <c r="E146" s="28"/>
+      <c r="F146" s="28"/>
     </row>
     <row r="147" spans="1:6" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="4" t="s">
@@ -11888,74 +12050,74 @@
       </c>
     </row>
     <row r="148" spans="1:6" ht="128.25" x14ac:dyDescent="0.25">
-      <c r="A148" s="21" t="s">
+      <c r="A148" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="B148" s="27" t="s">
+      <c r="B148" s="26" t="s">
         <v>104</v>
       </c>
       <c r="C148" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="D148" s="27" t="s">
+      <c r="D148" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="E148" s="27" t="s">
+      <c r="E148" s="26" t="s">
         <v>225</v>
       </c>
-      <c r="F148" s="27" t="s">
+      <c r="F148" s="26" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" s="22"/>
-      <c r="B149" s="28"/>
+      <c r="A149" s="30"/>
+      <c r="B149" s="27"/>
       <c r="C149" s="8"/>
-      <c r="D149" s="28"/>
-      <c r="E149" s="28"/>
-      <c r="F149" s="28"/>
+      <c r="D149" s="27"/>
+      <c r="E149" s="27"/>
+      <c r="F149" s="27"/>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A150" s="22"/>
-      <c r="B150" s="28"/>
+      <c r="A150" s="30"/>
+      <c r="B150" s="27"/>
       <c r="C150" s="8"/>
-      <c r="D150" s="28"/>
-      <c r="E150" s="28"/>
-      <c r="F150" s="28"/>
+      <c r="D150" s="27"/>
+      <c r="E150" s="27"/>
+      <c r="F150" s="27"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A151" s="22"/>
-      <c r="B151" s="28"/>
+      <c r="A151" s="30"/>
+      <c r="B151" s="27"/>
       <c r="C151" s="8"/>
-      <c r="D151" s="28"/>
-      <c r="E151" s="28"/>
-      <c r="F151" s="28"/>
+      <c r="D151" s="27"/>
+      <c r="E151" s="27"/>
+      <c r="F151" s="27"/>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A152" s="22"/>
-      <c r="B152" s="28"/>
+      <c r="A152" s="30"/>
+      <c r="B152" s="27"/>
       <c r="C152" s="8"/>
-      <c r="D152" s="28"/>
-      <c r="E152" s="28"/>
-      <c r="F152" s="28"/>
+      <c r="D152" s="27"/>
+      <c r="E152" s="27"/>
+      <c r="F152" s="27"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A153" s="22"/>
-      <c r="B153" s="28"/>
+      <c r="A153" s="30"/>
+      <c r="B153" s="27"/>
       <c r="C153" s="9"/>
-      <c r="D153" s="28"/>
-      <c r="E153" s="28"/>
-      <c r="F153" s="28"/>
+      <c r="D153" s="27"/>
+      <c r="E153" s="27"/>
+      <c r="F153" s="27"/>
     </row>
     <row r="154" spans="1:6" ht="114.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="23"/>
-      <c r="B154" s="29"/>
+      <c r="A154" s="31"/>
+      <c r="B154" s="28"/>
       <c r="C154" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="D154" s="29"/>
-      <c r="E154" s="29"/>
-      <c r="F154" s="29"/>
+      <c r="D154" s="28"/>
+      <c r="E154" s="28"/>
+      <c r="F154" s="28"/>
     </row>
     <row r="155" spans="1:6" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="4" t="s">
@@ -11981,47 +12143,47 @@
       <c r="A156" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="B156" s="27" t="s">
+      <c r="B156" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="C156" s="27" t="s">
+      <c r="C156" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="D156" s="27" t="s">
+      <c r="D156" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E156" s="27" t="s">
+      <c r="E156" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="F156" s="27" t="s">
+      <c r="F156" s="26" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="13"/>
-      <c r="B157" s="28"/>
-      <c r="C157" s="28"/>
-      <c r="D157" s="28"/>
-      <c r="E157" s="28"/>
-      <c r="F157" s="28"/>
+      <c r="B157" s="27"/>
+      <c r="C157" s="27"/>
+      <c r="D157" s="27"/>
+      <c r="E157" s="27"/>
+      <c r="F157" s="27"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="14"/>
-      <c r="B158" s="28"/>
-      <c r="C158" s="28"/>
-      <c r="D158" s="28"/>
-      <c r="E158" s="28"/>
-      <c r="F158" s="28"/>
+      <c r="B158" s="27"/>
+      <c r="C158" s="27"/>
+      <c r="D158" s="27"/>
+      <c r="E158" s="27"/>
+      <c r="F158" s="27"/>
     </row>
     <row r="159" spans="1:6" ht="42.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="B159" s="29"/>
-      <c r="C159" s="29"/>
-      <c r="D159" s="29"/>
-      <c r="E159" s="29"/>
-      <c r="F159" s="29"/>
+      <c r="B159" s="28"/>
+      <c r="C159" s="28"/>
+      <c r="D159" s="28"/>
+      <c r="E159" s="28"/>
+      <c r="F159" s="28"/>
     </row>
     <row r="160" spans="1:6" ht="243" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="4" t="s">
@@ -12084,82 +12246,82 @@
       </c>
     </row>
     <row r="163" spans="1:6" ht="57" x14ac:dyDescent="0.25">
-      <c r="A163" s="21" t="s">
+      <c r="A163" s="29" t="s">
         <v>241</v>
       </c>
       <c r="B163" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="C163" s="27" t="s">
+      <c r="C163" s="26" t="s">
         <v>244</v>
       </c>
-      <c r="D163" s="27" t="s">
+      <c r="D163" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E163" s="27" t="s">
+      <c r="E163" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F163" s="27" t="s">
+      <c r="F163" s="26" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A164" s="22"/>
+      <c r="A164" s="30"/>
       <c r="B164" s="8"/>
-      <c r="C164" s="28"/>
-      <c r="D164" s="28"/>
-      <c r="E164" s="28"/>
-      <c r="F164" s="28"/>
+      <c r="C164" s="27"/>
+      <c r="D164" s="27"/>
+      <c r="E164" s="27"/>
+      <c r="F164" s="27"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A165" s="22"/>
+      <c r="A165" s="30"/>
       <c r="B165" s="8"/>
-      <c r="C165" s="28"/>
-      <c r="D165" s="28"/>
-      <c r="E165" s="28"/>
-      <c r="F165" s="28"/>
+      <c r="C165" s="27"/>
+      <c r="D165" s="27"/>
+      <c r="E165" s="27"/>
+      <c r="F165" s="27"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A166" s="22"/>
+      <c r="A166" s="30"/>
       <c r="B166" s="8"/>
-      <c r="C166" s="28"/>
-      <c r="D166" s="28"/>
-      <c r="E166" s="28"/>
-      <c r="F166" s="28"/>
+      <c r="C166" s="27"/>
+      <c r="D166" s="27"/>
+      <c r="E166" s="27"/>
+      <c r="F166" s="27"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A167" s="22"/>
+      <c r="A167" s="30"/>
       <c r="B167" s="8"/>
-      <c r="C167" s="28"/>
-      <c r="D167" s="28"/>
-      <c r="E167" s="28"/>
-      <c r="F167" s="28"/>
+      <c r="C167" s="27"/>
+      <c r="D167" s="27"/>
+      <c r="E167" s="27"/>
+      <c r="F167" s="27"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A168" s="22"/>
+      <c r="A168" s="30"/>
       <c r="B168" s="8"/>
-      <c r="C168" s="28"/>
-      <c r="D168" s="28"/>
-      <c r="E168" s="28"/>
-      <c r="F168" s="28"/>
+      <c r="C168" s="27"/>
+      <c r="D168" s="27"/>
+      <c r="E168" s="27"/>
+      <c r="F168" s="27"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A169" s="22"/>
+      <c r="A169" s="30"/>
       <c r="B169" s="9"/>
-      <c r="C169" s="28"/>
-      <c r="D169" s="28"/>
-      <c r="E169" s="28"/>
-      <c r="F169" s="28"/>
+      <c r="C169" s="27"/>
+      <c r="D169" s="27"/>
+      <c r="E169" s="27"/>
+      <c r="F169" s="27"/>
     </row>
     <row r="170" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="23"/>
+      <c r="A170" s="31"/>
       <c r="B170" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="C170" s="29"/>
-      <c r="D170" s="29"/>
-      <c r="E170" s="29"/>
-      <c r="F170" s="29"/>
+      <c r="C170" s="28"/>
+      <c r="D170" s="28"/>
+      <c r="E170" s="28"/>
+      <c r="F170" s="28"/>
     </row>
     <row r="171" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="4" t="s">
@@ -12288,16 +12450,16 @@
       <c r="B177" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="C177" s="24" t="s">
+      <c r="C177" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="D177" s="27" t="s">
+      <c r="D177" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="E177" s="27" t="s">
+      <c r="E177" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F177" s="27" t="s">
+      <c r="F177" s="26" t="s">
         <v>44</v>
       </c>
     </row>
@@ -12306,194 +12468,194 @@
       <c r="B178" s="20" t="s">
         <v>266</v>
       </c>
-      <c r="C178" s="25"/>
-      <c r="D178" s="28"/>
-      <c r="E178" s="28"/>
-      <c r="F178" s="28"/>
+      <c r="C178" s="33"/>
+      <c r="D178" s="27"/>
+      <c r="E178" s="27"/>
+      <c r="F178" s="27"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="13"/>
       <c r="B179" s="9"/>
-      <c r="C179" s="25"/>
-      <c r="D179" s="28"/>
-      <c r="E179" s="28"/>
-      <c r="F179" s="28"/>
+      <c r="C179" s="33"/>
+      <c r="D179" s="27"/>
+      <c r="E179" s="27"/>
+      <c r="F179" s="27"/>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="13"/>
       <c r="B180" s="9"/>
-      <c r="C180" s="25"/>
-      <c r="D180" s="28"/>
-      <c r="E180" s="28"/>
-      <c r="F180" s="28"/>
+      <c r="C180" s="33"/>
+      <c r="D180" s="27"/>
+      <c r="E180" s="27"/>
+      <c r="F180" s="27"/>
     </row>
     <row r="181" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="16" t="s">
         <v>265</v>
       </c>
       <c r="B181" s="10"/>
-      <c r="C181" s="26"/>
-      <c r="D181" s="29"/>
-      <c r="E181" s="29"/>
-      <c r="F181" s="29"/>
+      <c r="C181" s="34"/>
+      <c r="D181" s="28"/>
+      <c r="E181" s="28"/>
+      <c r="F181" s="28"/>
     </row>
     <row r="182" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="B182" s="24" t="s">
+      <c r="B182" s="32" t="s">
         <v>271</v>
       </c>
-      <c r="C182" s="27" t="s">
+      <c r="C182" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D182" s="24" t="s">
+      <c r="D182" s="32" t="s">
         <v>191</v>
       </c>
-      <c r="E182" s="24" t="s">
+      <c r="E182" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="F182" s="24" t="s">
+      <c r="F182" s="32" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="13"/>
-      <c r="B183" s="25"/>
-      <c r="C183" s="28"/>
-      <c r="D183" s="25"/>
-      <c r="E183" s="25"/>
-      <c r="F183" s="25"/>
+      <c r="B183" s="33"/>
+      <c r="C183" s="27"/>
+      <c r="D183" s="33"/>
+      <c r="E183" s="33"/>
+      <c r="F183" s="33"/>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="13"/>
-      <c r="B184" s="25"/>
-      <c r="C184" s="28"/>
-      <c r="D184" s="25"/>
-      <c r="E184" s="25"/>
-      <c r="F184" s="25"/>
+      <c r="B184" s="33"/>
+      <c r="C184" s="27"/>
+      <c r="D184" s="33"/>
+      <c r="E184" s="33"/>
+      <c r="F184" s="33"/>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="13"/>
-      <c r="B185" s="25"/>
-      <c r="C185" s="28"/>
-      <c r="D185" s="25"/>
-      <c r="E185" s="25"/>
-      <c r="F185" s="25"/>
+      <c r="B185" s="33"/>
+      <c r="C185" s="27"/>
+      <c r="D185" s="33"/>
+      <c r="E185" s="33"/>
+      <c r="F185" s="33"/>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="13"/>
-      <c r="B186" s="25"/>
-      <c r="C186" s="28"/>
-      <c r="D186" s="25"/>
-      <c r="E186" s="25"/>
-      <c r="F186" s="25"/>
+      <c r="B186" s="33"/>
+      <c r="C186" s="27"/>
+      <c r="D186" s="33"/>
+      <c r="E186" s="33"/>
+      <c r="F186" s="33"/>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="13"/>
-      <c r="B187" s="25"/>
-      <c r="C187" s="28"/>
-      <c r="D187" s="25"/>
-      <c r="E187" s="25"/>
-      <c r="F187" s="25"/>
+      <c r="B187" s="33"/>
+      <c r="C187" s="27"/>
+      <c r="D187" s="33"/>
+      <c r="E187" s="33"/>
+      <c r="F187" s="33"/>
     </row>
     <row r="188" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A188" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="B188" s="25"/>
-      <c r="C188" s="28"/>
-      <c r="D188" s="25"/>
-      <c r="E188" s="25"/>
-      <c r="F188" s="25"/>
+      <c r="B188" s="33"/>
+      <c r="C188" s="27"/>
+      <c r="D188" s="33"/>
+      <c r="E188" s="33"/>
+      <c r="F188" s="33"/>
     </row>
     <row r="189" spans="1:6" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="B189" s="26"/>
-      <c r="C189" s="29"/>
-      <c r="D189" s="26"/>
-      <c r="E189" s="26"/>
-      <c r="F189" s="26"/>
+      <c r="B189" s="34"/>
+      <c r="C189" s="28"/>
+      <c r="D189" s="34"/>
+      <c r="E189" s="34"/>
+      <c r="F189" s="34"/>
     </row>
     <row r="190" spans="1:6" ht="57" x14ac:dyDescent="0.25">
-      <c r="A190" s="21" t="s">
+      <c r="A190" s="29" t="s">
         <v>273</v>
       </c>
       <c r="B190" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="C190" s="24" t="s">
+      <c r="C190" s="32" t="s">
         <v>276</v>
       </c>
-      <c r="D190" s="27" t="s">
+      <c r="D190" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="E190" s="27" t="s">
+      <c r="E190" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F190" s="27" t="s">
+      <c r="F190" s="26" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A191" s="22"/>
+      <c r="A191" s="30"/>
       <c r="B191" s="8"/>
-      <c r="C191" s="25"/>
-      <c r="D191" s="28"/>
-      <c r="E191" s="28"/>
-      <c r="F191" s="28"/>
+      <c r="C191" s="33"/>
+      <c r="D191" s="27"/>
+      <c r="E191" s="27"/>
+      <c r="F191" s="27"/>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A192" s="22"/>
+      <c r="A192" s="30"/>
       <c r="B192" s="8"/>
-      <c r="C192" s="25"/>
-      <c r="D192" s="28"/>
-      <c r="E192" s="28"/>
-      <c r="F192" s="28"/>
+      <c r="C192" s="33"/>
+      <c r="D192" s="27"/>
+      <c r="E192" s="27"/>
+      <c r="F192" s="27"/>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A193" s="22"/>
+      <c r="A193" s="30"/>
       <c r="B193" s="8"/>
-      <c r="C193" s="25"/>
-      <c r="D193" s="28"/>
-      <c r="E193" s="28"/>
-      <c r="F193" s="28"/>
+      <c r="C193" s="33"/>
+      <c r="D193" s="27"/>
+      <c r="E193" s="27"/>
+      <c r="F193" s="27"/>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A194" s="22"/>
+      <c r="A194" s="30"/>
       <c r="B194" s="8"/>
-      <c r="C194" s="25"/>
-      <c r="D194" s="28"/>
-      <c r="E194" s="28"/>
-      <c r="F194" s="28"/>
+      <c r="C194" s="33"/>
+      <c r="D194" s="27"/>
+      <c r="E194" s="27"/>
+      <c r="F194" s="27"/>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A195" s="22"/>
+      <c r="A195" s="30"/>
       <c r="B195" s="8"/>
-      <c r="C195" s="25"/>
-      <c r="D195" s="28"/>
-      <c r="E195" s="28"/>
-      <c r="F195" s="28"/>
+      <c r="C195" s="33"/>
+      <c r="D195" s="27"/>
+      <c r="E195" s="27"/>
+      <c r="F195" s="27"/>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A196" s="22"/>
+      <c r="A196" s="30"/>
       <c r="B196" s="9"/>
-      <c r="C196" s="25"/>
-      <c r="D196" s="28"/>
-      <c r="E196" s="28"/>
-      <c r="F196" s="28"/>
+      <c r="C196" s="33"/>
+      <c r="D196" s="27"/>
+      <c r="E196" s="27"/>
+      <c r="F196" s="27"/>
     </row>
     <row r="197" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A197" s="23"/>
+      <c r="A197" s="31"/>
       <c r="B197" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="C197" s="26"/>
-      <c r="D197" s="29"/>
-      <c r="E197" s="29"/>
-      <c r="F197" s="29"/>
+      <c r="C197" s="34"/>
+      <c r="D197" s="28"/>
+      <c r="E197" s="28"/>
+      <c r="F197" s="28"/>
     </row>
     <row r="198" spans="1:6" ht="114.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="4" t="s">
@@ -12602,16 +12764,16 @@
       <c r="B203" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="C203" s="27" t="s">
+      <c r="C203" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D203" s="27" t="s">
+      <c r="D203" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E203" s="27" t="s">
+      <c r="E203" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F203" s="27" t="s">
+      <c r="F203" s="26" t="s">
         <v>44</v>
       </c>
     </row>
@@ -12620,70 +12782,70 @@
       <c r="B204" s="20" t="s">
         <v>266</v>
       </c>
-      <c r="C204" s="28"/>
-      <c r="D204" s="28"/>
-      <c r="E204" s="28"/>
-      <c r="F204" s="28"/>
+      <c r="C204" s="27"/>
+      <c r="D204" s="27"/>
+      <c r="E204" s="27"/>
+      <c r="F204" s="27"/>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="13"/>
       <c r="B205" s="9"/>
-      <c r="C205" s="28"/>
-      <c r="D205" s="28"/>
-      <c r="E205" s="28"/>
-      <c r="F205" s="28"/>
+      <c r="C205" s="27"/>
+      <c r="D205" s="27"/>
+      <c r="E205" s="27"/>
+      <c r="F205" s="27"/>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="13"/>
       <c r="B206" s="9"/>
-      <c r="C206" s="28"/>
-      <c r="D206" s="28"/>
-      <c r="E206" s="28"/>
-      <c r="F206" s="28"/>
+      <c r="C206" s="27"/>
+      <c r="D206" s="27"/>
+      <c r="E206" s="27"/>
+      <c r="F206" s="27"/>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="13"/>
       <c r="B207" s="9"/>
-      <c r="C207" s="28"/>
-      <c r="D207" s="28"/>
-      <c r="E207" s="28"/>
-      <c r="F207" s="28"/>
+      <c r="C207" s="27"/>
+      <c r="D207" s="27"/>
+      <c r="E207" s="27"/>
+      <c r="F207" s="27"/>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="13"/>
       <c r="B208" s="9"/>
-      <c r="C208" s="28"/>
-      <c r="D208" s="28"/>
-      <c r="E208" s="28"/>
-      <c r="F208" s="28"/>
+      <c r="C208" s="27"/>
+      <c r="D208" s="27"/>
+      <c r="E208" s="27"/>
+      <c r="F208" s="27"/>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="13"/>
       <c r="B209" s="9"/>
-      <c r="C209" s="28"/>
-      <c r="D209" s="28"/>
-      <c r="E209" s="28"/>
-      <c r="F209" s="28"/>
+      <c r="C209" s="27"/>
+      <c r="D209" s="27"/>
+      <c r="E209" s="27"/>
+      <c r="F209" s="27"/>
     </row>
     <row r="210" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A210" s="14" t="s">
         <v>288</v>
       </c>
       <c r="B210" s="9"/>
-      <c r="C210" s="28"/>
-      <c r="D210" s="28"/>
-      <c r="E210" s="28"/>
-      <c r="F210" s="28"/>
+      <c r="C210" s="27"/>
+      <c r="D210" s="27"/>
+      <c r="E210" s="27"/>
+      <c r="F210" s="27"/>
     </row>
     <row r="211" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="16" t="s">
         <v>289</v>
       </c>
       <c r="B211" s="10"/>
-      <c r="C211" s="29"/>
-      <c r="D211" s="29"/>
-      <c r="E211" s="29"/>
-      <c r="F211" s="29"/>
+      <c r="C211" s="28"/>
+      <c r="D211" s="28"/>
+      <c r="E211" s="28"/>
+      <c r="F211" s="28"/>
     </row>
     <row r="212" spans="1:6" ht="114.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="4" t="s">
@@ -12786,120 +12948,120 @@
       </c>
     </row>
     <row r="217" spans="1:6" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="A217" s="21" t="s">
+      <c r="A217" s="29" t="s">
         <v>304</v>
       </c>
       <c r="B217" s="11" t="s">
         <v>305</v>
       </c>
-      <c r="C217" s="27" t="s">
+      <c r="C217" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D217" s="27" t="s">
+      <c r="D217" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="E217" s="27" t="s">
+      <c r="E217" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F217" s="27" t="s">
+      <c r="F217" s="26" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A218" s="22"/>
+      <c r="A218" s="30"/>
       <c r="B218" s="8"/>
-      <c r="C218" s="28"/>
-      <c r="D218" s="28"/>
-      <c r="E218" s="28"/>
-      <c r="F218" s="28"/>
+      <c r="C218" s="27"/>
+      <c r="D218" s="27"/>
+      <c r="E218" s="27"/>
+      <c r="F218" s="27"/>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A219" s="22"/>
+      <c r="A219" s="30"/>
       <c r="B219" s="8"/>
-      <c r="C219" s="28"/>
-      <c r="D219" s="28"/>
-      <c r="E219" s="28"/>
-      <c r="F219" s="28"/>
+      <c r="C219" s="27"/>
+      <c r="D219" s="27"/>
+      <c r="E219" s="27"/>
+      <c r="F219" s="27"/>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A220" s="22"/>
+      <c r="A220" s="30"/>
       <c r="B220" s="8"/>
-      <c r="C220" s="28"/>
-      <c r="D220" s="28"/>
-      <c r="E220" s="28"/>
-      <c r="F220" s="28"/>
+      <c r="C220" s="27"/>
+      <c r="D220" s="27"/>
+      <c r="E220" s="27"/>
+      <c r="F220" s="27"/>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A221" s="22"/>
+      <c r="A221" s="30"/>
       <c r="B221" s="9"/>
-      <c r="C221" s="28"/>
-      <c r="D221" s="28"/>
-      <c r="E221" s="28"/>
-      <c r="F221" s="28"/>
+      <c r="C221" s="27"/>
+      <c r="D221" s="27"/>
+      <c r="E221" s="27"/>
+      <c r="F221" s="27"/>
     </row>
     <row r="222" spans="1:6" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A222" s="23"/>
+      <c r="A222" s="31"/>
       <c r="B222" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="C222" s="29"/>
-      <c r="D222" s="29"/>
-      <c r="E222" s="29"/>
-      <c r="F222" s="29"/>
+      <c r="C222" s="28"/>
+      <c r="D222" s="28"/>
+      <c r="E222" s="28"/>
+      <c r="F222" s="28"/>
     </row>
     <row r="223" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A223" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="B223" s="30" t="s">
+      <c r="B223" s="23" t="s">
         <v>310</v>
       </c>
-      <c r="C223" s="27" t="s">
+      <c r="C223" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D223" s="27" t="s">
+      <c r="D223" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="E223" s="27" t="s">
+      <c r="E223" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="F223" s="27" t="s">
+      <c r="F223" s="26" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="13"/>
-      <c r="B224" s="31"/>
-      <c r="C224" s="28"/>
-      <c r="D224" s="28"/>
-      <c r="E224" s="28"/>
-      <c r="F224" s="28"/>
+      <c r="B224" s="24"/>
+      <c r="C224" s="27"/>
+      <c r="D224" s="27"/>
+      <c r="E224" s="27"/>
+      <c r="F224" s="27"/>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="13"/>
-      <c r="B225" s="31"/>
-      <c r="C225" s="28"/>
-      <c r="D225" s="28"/>
-      <c r="E225" s="28"/>
-      <c r="F225" s="28"/>
+      <c r="B225" s="24"/>
+      <c r="C225" s="27"/>
+      <c r="D225" s="27"/>
+      <c r="E225" s="27"/>
+      <c r="F225" s="27"/>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="18"/>
-      <c r="B226" s="31"/>
-      <c r="C226" s="28"/>
-      <c r="D226" s="28"/>
-      <c r="E226" s="28"/>
-      <c r="F226" s="28"/>
+      <c r="B226" s="24"/>
+      <c r="C226" s="27"/>
+      <c r="D226" s="27"/>
+      <c r="E226" s="27"/>
+      <c r="F226" s="27"/>
     </row>
     <row r="227" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="B227" s="32"/>
-      <c r="C227" s="29"/>
-      <c r="D227" s="29"/>
-      <c r="E227" s="29"/>
-      <c r="F227" s="29"/>
+      <c r="B227" s="25"/>
+      <c r="C227" s="28"/>
+      <c r="D227" s="28"/>
+      <c r="E227" s="28"/>
+      <c r="F227" s="28"/>
     </row>
     <row r="228" spans="1:6" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="4" t="s">
@@ -12943,74 +13105,46 @@
     </row>
   </sheetData>
   <mergeCells count="122">
-    <mergeCell ref="B223:B227"/>
-    <mergeCell ref="C223:C227"/>
-    <mergeCell ref="D223:D227"/>
-    <mergeCell ref="E223:E227"/>
-    <mergeCell ref="F223:F227"/>
-    <mergeCell ref="C203:C211"/>
-    <mergeCell ref="D203:D211"/>
-    <mergeCell ref="E203:E211"/>
-    <mergeCell ref="F203:F211"/>
-    <mergeCell ref="A217:A222"/>
-    <mergeCell ref="C217:C222"/>
-    <mergeCell ref="D217:D222"/>
-    <mergeCell ref="E217:E222"/>
-    <mergeCell ref="F217:F222"/>
-    <mergeCell ref="A190:A197"/>
-    <mergeCell ref="C190:C197"/>
-    <mergeCell ref="D190:D197"/>
-    <mergeCell ref="E190:E197"/>
-    <mergeCell ref="F190:F197"/>
-    <mergeCell ref="C177:C181"/>
-    <mergeCell ref="D177:D181"/>
-    <mergeCell ref="E177:E181"/>
-    <mergeCell ref="F177:F181"/>
-    <mergeCell ref="B182:B189"/>
-    <mergeCell ref="C182:C189"/>
-    <mergeCell ref="D182:D189"/>
-    <mergeCell ref="E182:E189"/>
-    <mergeCell ref="F182:F189"/>
-    <mergeCell ref="A163:A170"/>
-    <mergeCell ref="C163:C170"/>
-    <mergeCell ref="D163:D170"/>
-    <mergeCell ref="E163:E170"/>
-    <mergeCell ref="F163:F170"/>
-    <mergeCell ref="B156:B159"/>
-    <mergeCell ref="C156:C159"/>
-    <mergeCell ref="D156:D159"/>
-    <mergeCell ref="E156:E159"/>
-    <mergeCell ref="F156:F159"/>
-    <mergeCell ref="A148:A154"/>
-    <mergeCell ref="B148:B154"/>
-    <mergeCell ref="D148:D154"/>
-    <mergeCell ref="E148:E154"/>
-    <mergeCell ref="F148:F154"/>
-    <mergeCell ref="A142:A146"/>
-    <mergeCell ref="C142:C146"/>
-    <mergeCell ref="D142:D146"/>
-    <mergeCell ref="E142:E146"/>
-    <mergeCell ref="F142:F146"/>
-    <mergeCell ref="A131:A141"/>
-    <mergeCell ref="C131:C141"/>
-    <mergeCell ref="D131:D141"/>
-    <mergeCell ref="E131:E141"/>
-    <mergeCell ref="F131:F141"/>
-    <mergeCell ref="A122:A130"/>
-    <mergeCell ref="C122:C130"/>
-    <mergeCell ref="D122:D130"/>
-    <mergeCell ref="E122:E130"/>
-    <mergeCell ref="F122:F130"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="C120:C121"/>
-    <mergeCell ref="D120:D121"/>
-    <mergeCell ref="E120:E121"/>
-    <mergeCell ref="F120:F121"/>
-    <mergeCell ref="B112:B119"/>
-    <mergeCell ref="C112:C119"/>
-    <mergeCell ref="D112:D119"/>
-    <mergeCell ref="E112:E119"/>
-    <mergeCell ref="F112:F119"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="A13:A18"/>
+    <mergeCell ref="C13:C18"/>
+    <mergeCell ref="D13:D18"/>
+    <mergeCell ref="E13:E18"/>
+    <mergeCell ref="F13:F18"/>
+    <mergeCell ref="A42:A47"/>
+    <mergeCell ref="C42:C47"/>
+    <mergeCell ref="D42:D47"/>
+    <mergeCell ref="E42:E47"/>
+    <mergeCell ref="F42:F47"/>
+    <mergeCell ref="A24:A30"/>
+    <mergeCell ref="C24:C30"/>
+    <mergeCell ref="D24:D30"/>
+    <mergeCell ref="E24:E30"/>
+    <mergeCell ref="F24:F30"/>
+    <mergeCell ref="B56:B61"/>
+    <mergeCell ref="C56:C61"/>
+    <mergeCell ref="D56:D61"/>
+    <mergeCell ref="E56:E61"/>
+    <mergeCell ref="F56:F61"/>
+    <mergeCell ref="B51:B55"/>
+    <mergeCell ref="C51:C55"/>
+    <mergeCell ref="D51:D55"/>
+    <mergeCell ref="E51:E55"/>
+    <mergeCell ref="F51:F55"/>
+    <mergeCell ref="B74:B78"/>
+    <mergeCell ref="C74:C78"/>
+    <mergeCell ref="D74:D78"/>
+    <mergeCell ref="E74:E78"/>
+    <mergeCell ref="F74:F78"/>
+    <mergeCell ref="A68:A72"/>
+    <mergeCell ref="C68:C72"/>
+    <mergeCell ref="D68:D72"/>
+    <mergeCell ref="E68:E72"/>
+    <mergeCell ref="F68:F72"/>
     <mergeCell ref="A100:A103"/>
     <mergeCell ref="C100:C103"/>
     <mergeCell ref="D100:D103"/>
@@ -13025,46 +13159,74 @@
     <mergeCell ref="D90:D94"/>
     <mergeCell ref="E90:E94"/>
     <mergeCell ref="F90:F94"/>
-    <mergeCell ref="B74:B78"/>
-    <mergeCell ref="C74:C78"/>
-    <mergeCell ref="D74:D78"/>
-    <mergeCell ref="E74:E78"/>
-    <mergeCell ref="F74:F78"/>
-    <mergeCell ref="A68:A72"/>
-    <mergeCell ref="C68:C72"/>
-    <mergeCell ref="D68:D72"/>
-    <mergeCell ref="E68:E72"/>
-    <mergeCell ref="F68:F72"/>
-    <mergeCell ref="B56:B61"/>
-    <mergeCell ref="C56:C61"/>
-    <mergeCell ref="D56:D61"/>
-    <mergeCell ref="E56:E61"/>
-    <mergeCell ref="F56:F61"/>
-    <mergeCell ref="B51:B55"/>
-    <mergeCell ref="C51:C55"/>
-    <mergeCell ref="D51:D55"/>
-    <mergeCell ref="E51:E55"/>
-    <mergeCell ref="F51:F55"/>
-    <mergeCell ref="A42:A47"/>
-    <mergeCell ref="C42:C47"/>
-    <mergeCell ref="D42:D47"/>
-    <mergeCell ref="E42:E47"/>
-    <mergeCell ref="F42:F47"/>
-    <mergeCell ref="A24:A30"/>
-    <mergeCell ref="C24:C30"/>
-    <mergeCell ref="D24:D30"/>
-    <mergeCell ref="E24:E30"/>
-    <mergeCell ref="F24:F30"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="C13:C18"/>
-    <mergeCell ref="D13:D18"/>
-    <mergeCell ref="E13:E18"/>
-    <mergeCell ref="F13:F18"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="C120:C121"/>
+    <mergeCell ref="D120:D121"/>
+    <mergeCell ref="E120:E121"/>
+    <mergeCell ref="F120:F121"/>
+    <mergeCell ref="B112:B119"/>
+    <mergeCell ref="C112:C119"/>
+    <mergeCell ref="D112:D119"/>
+    <mergeCell ref="E112:E119"/>
+    <mergeCell ref="F112:F119"/>
+    <mergeCell ref="A131:A141"/>
+    <mergeCell ref="C131:C141"/>
+    <mergeCell ref="D131:D141"/>
+    <mergeCell ref="E131:E141"/>
+    <mergeCell ref="F131:F141"/>
+    <mergeCell ref="A122:A130"/>
+    <mergeCell ref="C122:C130"/>
+    <mergeCell ref="D122:D130"/>
+    <mergeCell ref="E122:E130"/>
+    <mergeCell ref="F122:F130"/>
+    <mergeCell ref="A148:A154"/>
+    <mergeCell ref="B148:B154"/>
+    <mergeCell ref="D148:D154"/>
+    <mergeCell ref="E148:E154"/>
+    <mergeCell ref="F148:F154"/>
+    <mergeCell ref="A142:A146"/>
+    <mergeCell ref="C142:C146"/>
+    <mergeCell ref="D142:D146"/>
+    <mergeCell ref="E142:E146"/>
+    <mergeCell ref="F142:F146"/>
+    <mergeCell ref="A163:A170"/>
+    <mergeCell ref="C163:C170"/>
+    <mergeCell ref="D163:D170"/>
+    <mergeCell ref="E163:E170"/>
+    <mergeCell ref="F163:F170"/>
+    <mergeCell ref="B156:B159"/>
+    <mergeCell ref="C156:C159"/>
+    <mergeCell ref="D156:D159"/>
+    <mergeCell ref="E156:E159"/>
+    <mergeCell ref="F156:F159"/>
+    <mergeCell ref="C177:C181"/>
+    <mergeCell ref="D177:D181"/>
+    <mergeCell ref="E177:E181"/>
+    <mergeCell ref="F177:F181"/>
+    <mergeCell ref="B182:B189"/>
+    <mergeCell ref="C182:C189"/>
+    <mergeCell ref="D182:D189"/>
+    <mergeCell ref="E182:E189"/>
+    <mergeCell ref="F182:F189"/>
+    <mergeCell ref="A217:A222"/>
+    <mergeCell ref="C217:C222"/>
+    <mergeCell ref="D217:D222"/>
+    <mergeCell ref="E217:E222"/>
+    <mergeCell ref="F217:F222"/>
+    <mergeCell ref="A190:A197"/>
+    <mergeCell ref="C190:C197"/>
+    <mergeCell ref="D190:D197"/>
+    <mergeCell ref="E190:E197"/>
+    <mergeCell ref="F190:F197"/>
+    <mergeCell ref="B223:B227"/>
+    <mergeCell ref="C223:C227"/>
+    <mergeCell ref="D223:D227"/>
+    <mergeCell ref="E223:E227"/>
+    <mergeCell ref="F223:F227"/>
+    <mergeCell ref="C203:C211"/>
+    <mergeCell ref="D203:D211"/>
+    <mergeCell ref="E203:E211"/>
+    <mergeCell ref="F203:F211"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" tooltip="Aegean cat" display="https://en.wikipedia.org/wiki/Aegean_cat" xr:uid="{6703FBD1-88B6-4565-9001-B3C67A67739E}"/>
@@ -13256,10 +13418,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E730C0B2-6DE9-4F50-AD37-39852B7F947B}">
-  <dimension ref="B1:S123"/>
+  <dimension ref="B1:S152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J60" sqref="J60:K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13268,7 +13430,7 @@
     <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="37" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" customWidth="1"/>
@@ -13284,7 +13446,7 @@
       <c r="C1">
         <v>1</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="22" t="s">
         <v>360</v>
       </c>
       <c r="G1" t="s">
@@ -13293,7 +13455,7 @@
       <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="21" t="s">
         <v>15</v>
       </c>
       <c r="M1" t="s">
@@ -13313,7 +13475,7 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="22" t="s">
         <v>361</v>
       </c>
       <c r="G2" t="s">
@@ -13322,7 +13484,7 @@
       <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="21" t="s">
         <v>218</v>
       </c>
       <c r="M2">
@@ -13342,7 +13504,7 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="22" t="s">
         <v>339</v>
       </c>
       <c r="G3" t="s">
@@ -13351,7 +13513,7 @@
       <c r="I3" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="36" t="s">
+      <c r="K3" s="21" t="s">
         <v>174</v>
       </c>
       <c r="M3">
@@ -13371,7 +13533,7 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="22" t="s">
         <v>66</v>
       </c>
       <c r="G4" t="s">
@@ -13380,7 +13542,7 @@
       <c r="I4" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="36" t="s">
+      <c r="K4" s="21" t="s">
         <v>33</v>
       </c>
       <c r="M4">
@@ -13400,7 +13562,7 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="22" t="s">
         <v>353</v>
       </c>
       <c r="G5" t="s">
@@ -13409,7 +13571,7 @@
       <c r="I5" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="36" t="s">
+      <c r="K5" s="21" t="s">
         <v>335</v>
       </c>
       <c r="M5">
@@ -13429,7 +13591,7 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="22" t="s">
         <v>340</v>
       </c>
       <c r="G6" t="s">
@@ -13438,7 +13600,7 @@
       <c r="I6" t="s">
         <v>105</v>
       </c>
-      <c r="K6" s="36" t="s">
+      <c r="K6" s="21" t="s">
         <v>206</v>
       </c>
       <c r="M6">
@@ -13458,7 +13620,7 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="22" t="s">
         <v>119</v>
       </c>
       <c r="G7" t="s">
@@ -13467,7 +13629,7 @@
       <c r="I7" t="s">
         <v>364</v>
       </c>
-      <c r="K7" s="36" t="s">
+      <c r="K7" s="21" t="s">
         <v>334</v>
       </c>
       <c r="M7">
@@ -13487,7 +13649,7 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="22" t="s">
         <v>109</v>
       </c>
       <c r="G8" t="s">
@@ -13496,7 +13658,7 @@
       <c r="I8" t="s">
         <v>365</v>
       </c>
-      <c r="K8" s="36" t="s">
+      <c r="K8" s="21" t="s">
         <v>387</v>
       </c>
       <c r="M8">
@@ -13516,7 +13678,7 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="22" t="s">
         <v>347</v>
       </c>
       <c r="G9" t="s">
@@ -13525,7 +13687,7 @@
       <c r="I9" t="s">
         <v>366</v>
       </c>
-      <c r="K9" s="36" t="s">
+      <c r="K9" s="21" t="s">
         <v>170</v>
       </c>
       <c r="M9">
@@ -13545,7 +13707,7 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="22" t="s">
         <v>354</v>
       </c>
       <c r="G10" t="s">
@@ -13554,7 +13716,7 @@
       <c r="I10" t="s">
         <v>169</v>
       </c>
-      <c r="K10" s="36" t="s">
+      <c r="K10" s="21" t="s">
         <v>388</v>
       </c>
       <c r="M10">
@@ -13574,13 +13736,13 @@
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="22" t="s">
         <v>25</v>
       </c>
       <c r="G11" t="s">
         <v>337</v>
       </c>
-      <c r="K11" s="36" t="s">
+      <c r="K11" s="21" t="s">
         <v>389</v>
       </c>
       <c r="M11">
@@ -13600,13 +13762,13 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="E12" s="37" t="s">
+      <c r="E12" s="22" t="s">
         <v>352</v>
       </c>
       <c r="G12" t="s">
         <v>141</v>
       </c>
-      <c r="K12" s="36" t="s">
+      <c r="K12" s="21" t="s">
         <v>406</v>
       </c>
       <c r="M12">
@@ -13626,13 +13788,13 @@
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="E13" s="37" t="s">
+      <c r="E13" s="22" t="s">
         <v>362</v>
       </c>
       <c r="G13" t="s">
         <v>160</v>
       </c>
-      <c r="K13" s="36" t="s">
+      <c r="K13" s="21" t="s">
         <v>390</v>
       </c>
       <c r="M13">
@@ -13652,13 +13814,13 @@
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="E14" s="22" t="s">
         <v>343</v>
       </c>
       <c r="G14" t="s">
         <v>228</v>
       </c>
-      <c r="K14" s="36" t="s">
+      <c r="K14" s="21" t="s">
         <v>391</v>
       </c>
       <c r="M14">
@@ -13678,10 +13840,13 @@
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="E15" s="37" t="s">
+      <c r="E15" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="K15" s="36" t="s">
+      <c r="G15" t="s">
+        <v>448</v>
+      </c>
+      <c r="K15" s="21" t="s">
         <v>392</v>
       </c>
       <c r="M15">
@@ -13701,10 +13866,10 @@
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="E16" s="37" t="s">
+      <c r="E16" s="22" t="s">
         <v>363</v>
       </c>
-      <c r="K16" s="36" t="s">
+      <c r="K16" s="21" t="s">
         <v>393</v>
       </c>
       <c r="M16">
@@ -13724,10 +13889,10 @@
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="E17" s="37" t="s">
+      <c r="E17" s="22" t="s">
         <v>342</v>
       </c>
-      <c r="K17" s="36" t="s">
+      <c r="K17" s="21" t="s">
         <v>44</v>
       </c>
       <c r="M17">
@@ -13747,10 +13912,10 @@
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="E18" s="37" t="s">
+      <c r="E18" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="K18" s="36" t="s">
+      <c r="K18" s="21" t="s">
         <v>394</v>
       </c>
       <c r="M18">
@@ -13770,10 +13935,10 @@
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="E19" s="37" t="s">
+      <c r="E19" s="22" t="s">
         <v>359</v>
       </c>
-      <c r="K19" s="36" t="s">
+      <c r="K19" s="21" t="s">
         <v>301</v>
       </c>
       <c r="M19">
@@ -13793,10 +13958,10 @@
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="E20" s="37" t="s">
+      <c r="E20" s="22" t="s">
         <v>346</v>
       </c>
-      <c r="K20" s="36" t="s">
+      <c r="K20" s="21" t="s">
         <v>395</v>
       </c>
       <c r="M20">
@@ -13816,10 +13981,10 @@
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="E21" s="37" t="s">
+      <c r="E21" s="22" t="s">
         <v>348</v>
       </c>
-      <c r="K21" s="36" t="s">
+      <c r="K21" s="21" t="s">
         <v>396</v>
       </c>
       <c r="M21">
@@ -13839,10 +14004,10 @@
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="E22" s="37" t="s">
+      <c r="E22" s="22" t="s">
         <v>344</v>
       </c>
-      <c r="K22" s="36" t="s">
+      <c r="K22" s="21" t="s">
         <v>330</v>
       </c>
       <c r="M22">
@@ -13862,10 +14027,10 @@
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="E23" s="37" t="s">
+      <c r="E23" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="K23" s="36" t="s">
+      <c r="K23" s="21" t="s">
         <v>60</v>
       </c>
       <c r="M23">
@@ -13885,10 +14050,10 @@
       <c r="C24">
         <v>1</v>
       </c>
-      <c r="E24" s="37" t="s">
+      <c r="E24" s="22" t="s">
         <v>350</v>
       </c>
-      <c r="K24" s="36" t="s">
+      <c r="K24" s="21" t="s">
         <v>10</v>
       </c>
       <c r="M24">
@@ -13908,10 +14073,10 @@
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="E25" s="37" t="s">
+      <c r="E25" s="22" t="s">
         <v>351</v>
       </c>
-      <c r="K25" s="36" t="s">
+      <c r="K25" s="21" t="s">
         <v>407</v>
       </c>
       <c r="M25">
@@ -13931,10 +14096,10 @@
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="E26" s="37" t="s">
+      <c r="E26" s="22" t="s">
         <v>349</v>
       </c>
-      <c r="K26" s="36" t="s">
+      <c r="K26" s="21" t="s">
         <v>397</v>
       </c>
       <c r="M26">
@@ -13954,10 +14119,10 @@
       <c r="C27">
         <v>1</v>
       </c>
-      <c r="E27" s="37" t="s">
+      <c r="E27" s="22" t="s">
         <v>358</v>
       </c>
-      <c r="K27" s="36" t="s">
+      <c r="K27" s="21" t="s">
         <v>398</v>
       </c>
       <c r="M27">
@@ -13977,10 +14142,10 @@
       <c r="C28">
         <v>1</v>
       </c>
-      <c r="E28" s="37" t="s">
+      <c r="E28" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="K28" s="36" t="s">
+      <c r="K28" s="21" t="s">
         <v>106</v>
       </c>
       <c r="M28">
@@ -14000,10 +14165,10 @@
       <c r="C29">
         <v>1</v>
       </c>
-      <c r="E29" s="37" t="s">
+      <c r="E29" s="22" t="s">
         <v>356</v>
       </c>
-      <c r="K29" s="36" t="s">
+      <c r="K29" s="21" t="s">
         <v>64</v>
       </c>
       <c r="M29">
@@ -14023,10 +14188,10 @@
       <c r="C30">
         <v>1</v>
       </c>
-      <c r="E30" s="37" t="s">
+      <c r="E30" s="22" t="s">
         <v>357</v>
       </c>
-      <c r="K30" s="36" t="s">
+      <c r="K30" s="21" t="s">
         <v>154</v>
       </c>
       <c r="M30">
@@ -14046,10 +14211,10 @@
       <c r="C31">
         <v>1</v>
       </c>
-      <c r="E31" s="37" t="s">
+      <c r="E31" s="22" t="s">
         <v>345</v>
       </c>
-      <c r="K31" s="36" t="s">
+      <c r="K31" s="21" t="s">
         <v>126</v>
       </c>
       <c r="M31">
@@ -14069,10 +14234,10 @@
       <c r="C32">
         <v>1</v>
       </c>
-      <c r="E32" s="37" t="s">
+      <c r="E32" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="K32" s="36" t="s">
+      <c r="K32" s="21" t="s">
         <v>333</v>
       </c>
       <c r="M32">
@@ -14092,10 +14257,10 @@
       <c r="C33">
         <v>1</v>
       </c>
-      <c r="E33" s="37" t="s">
+      <c r="E33" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="K33" s="36" t="s">
+      <c r="K33" s="21" t="s">
         <v>399</v>
       </c>
       <c r="M33">
@@ -14115,10 +14280,10 @@
       <c r="C34">
         <v>1</v>
       </c>
-      <c r="E34" s="37" t="s">
+      <c r="E34" s="22" t="s">
         <v>341</v>
       </c>
-      <c r="K34" s="36" t="s">
+      <c r="K34" s="21" t="s">
         <v>315</v>
       </c>
       <c r="M34">
@@ -14138,10 +14303,10 @@
       <c r="C35">
         <v>1</v>
       </c>
-      <c r="E35" s="37" t="s">
+      <c r="E35" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="K35" s="36" t="s">
+      <c r="K35" s="21" t="s">
         <v>332</v>
       </c>
       <c r="M35">
@@ -14161,10 +14326,10 @@
       <c r="C36">
         <v>1</v>
       </c>
-      <c r="E36" s="37" t="s">
+      <c r="E36" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="K36" s="36" t="s">
+      <c r="K36" s="21" t="s">
         <v>400</v>
       </c>
       <c r="M36">
@@ -14184,10 +14349,10 @@
       <c r="C37">
         <v>1</v>
       </c>
-      <c r="E37" s="37" t="s">
+      <c r="E37" s="22" t="s">
         <v>355</v>
       </c>
-      <c r="K37" s="36" t="s">
+      <c r="K37" s="21" t="s">
         <v>286</v>
       </c>
       <c r="M37">
@@ -14207,10 +14372,10 @@
       <c r="C38">
         <v>1</v>
       </c>
-      <c r="E38" s="37" t="s">
+      <c r="E38" s="22" t="s">
         <v>313</v>
       </c>
-      <c r="K38" s="36" t="s">
+      <c r="K38" s="21" t="s">
         <v>331</v>
       </c>
       <c r="M38">
@@ -14230,7 +14395,10 @@
       <c r="C39">
         <v>1</v>
       </c>
-      <c r="K39" s="36" t="s">
+      <c r="E39" s="22" t="s">
+        <v>447</v>
+      </c>
+      <c r="K39" s="21" t="s">
         <v>401</v>
       </c>
       <c r="M39">
@@ -14250,7 +14418,10 @@
       <c r="C40">
         <v>1</v>
       </c>
-      <c r="K40" s="36" t="s">
+      <c r="E40" s="22" t="s">
+        <v>449</v>
+      </c>
+      <c r="K40" s="21" t="s">
         <v>148</v>
       </c>
       <c r="M40">
@@ -14270,7 +14441,10 @@
       <c r="C41">
         <v>1</v>
       </c>
-      <c r="K41" s="36" t="s">
+      <c r="E41" s="22" t="s">
+        <v>450</v>
+      </c>
+      <c r="K41" s="21" t="s">
         <v>402</v>
       </c>
       <c r="M41">
@@ -14290,7 +14464,7 @@
       <c r="C42">
         <v>1</v>
       </c>
-      <c r="K42" s="36" t="s">
+      <c r="K42" s="21" t="s">
         <v>250</v>
       </c>
       <c r="M42">
@@ -14310,7 +14484,7 @@
       <c r="C43">
         <v>1</v>
       </c>
-      <c r="K43" s="36" t="s">
+      <c r="K43" s="21" t="s">
         <v>38</v>
       </c>
       <c r="M43">
@@ -14330,7 +14504,7 @@
       <c r="C44">
         <v>1</v>
       </c>
-      <c r="K44" s="36" t="s">
+      <c r="K44" s="21" t="s">
         <v>81</v>
       </c>
       <c r="M44">
@@ -14350,7 +14524,7 @@
       <c r="C45">
         <v>1</v>
       </c>
-      <c r="K45" s="36" t="s">
+      <c r="K45" s="21" t="s">
         <v>403</v>
       </c>
       <c r="M45">
@@ -14370,7 +14544,7 @@
       <c r="C46">
         <v>1</v>
       </c>
-      <c r="K46" s="36" t="s">
+      <c r="K46" s="21" t="s">
         <v>5</v>
       </c>
       <c r="M46">
@@ -14390,7 +14564,7 @@
       <c r="C47">
         <v>1</v>
       </c>
-      <c r="K47" s="36" t="s">
+      <c r="K47" s="21" t="s">
         <v>336</v>
       </c>
       <c r="M47">
@@ -14410,7 +14584,7 @@
       <c r="C48">
         <v>1</v>
       </c>
-      <c r="K48" s="36" t="s">
+      <c r="K48" s="21" t="s">
         <v>307</v>
       </c>
       <c r="M48">
@@ -14430,7 +14604,7 @@
       <c r="C49">
         <v>1</v>
       </c>
-      <c r="K49" s="36" t="s">
+      <c r="K49" s="21" t="s">
         <v>88</v>
       </c>
       <c r="M49">
@@ -14450,7 +14624,7 @@
       <c r="C50">
         <v>1</v>
       </c>
-      <c r="K50" s="36" t="s">
+      <c r="K50" s="21" t="s">
         <v>404</v>
       </c>
       <c r="M50">
@@ -14496,6 +14670,9 @@
       <c r="C52">
         <v>1</v>
       </c>
+      <c r="K52" t="s">
+        <v>451</v>
+      </c>
       <c r="M52">
         <v>51</v>
       </c>
@@ -14513,6 +14690,9 @@
       <c r="C53">
         <v>1</v>
       </c>
+      <c r="K53" t="s">
+        <v>452</v>
+      </c>
       <c r="M53">
         <v>52</v>
       </c>
@@ -14530,6 +14710,9 @@
       <c r="C54">
         <v>1</v>
       </c>
+      <c r="K54" t="s">
+        <v>453</v>
+      </c>
       <c r="M54">
         <v>53</v>
       </c>
@@ -14547,6 +14730,9 @@
       <c r="C55">
         <v>1</v>
       </c>
+      <c r="K55" t="s">
+        <v>454</v>
+      </c>
       <c r="M55">
         <v>54</v>
       </c>
@@ -14561,6 +14747,9 @@
       <c r="C56">
         <v>1</v>
       </c>
+      <c r="K56" t="s">
+        <v>455</v>
+      </c>
       <c r="M56">
         <v>55</v>
       </c>
@@ -14578,6 +14767,9 @@
       <c r="C57">
         <v>1</v>
       </c>
+      <c r="K57" t="s">
+        <v>456</v>
+      </c>
       <c r="M57">
         <v>56</v>
       </c>
@@ -14595,6 +14787,9 @@
       <c r="C58">
         <v>1</v>
       </c>
+      <c r="K58" t="s">
+        <v>457</v>
+      </c>
       <c r="M58">
         <v>57</v>
       </c>
@@ -14612,6 +14807,9 @@
       <c r="C59">
         <v>1</v>
       </c>
+      <c r="K59" t="s">
+        <v>458</v>
+      </c>
       <c r="M59">
         <v>58</v>
       </c>
@@ -14629,6 +14827,9 @@
       <c r="C60">
         <v>1</v>
       </c>
+      <c r="K60" t="s">
+        <v>459</v>
+      </c>
       <c r="M60">
         <v>59</v>
       </c>
@@ -14646,6 +14847,9 @@
       <c r="C61">
         <v>1</v>
       </c>
+      <c r="K61" t="s">
+        <v>460</v>
+      </c>
       <c r="M61">
         <v>60</v>
       </c>
@@ -14663,6 +14867,9 @@
       <c r="C62">
         <v>1</v>
       </c>
+      <c r="K62" t="s">
+        <v>461</v>
+      </c>
       <c r="M62">
         <v>61</v>
       </c>
@@ -15490,6 +15697,9 @@
       </c>
     </row>
     <row r="111" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>308</v>
+      </c>
       <c r="C111">
         <v>1</v>
       </c>
@@ -15538,6 +15748,12 @@
       </c>
     </row>
     <row r="114" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>408</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
       <c r="M114">
         <v>115</v>
       </c>
@@ -15549,6 +15765,12 @@
       </c>
     </row>
     <row r="115" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>409</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
       <c r="M115">
         <v>116</v>
       </c>
@@ -15560,6 +15782,12 @@
       </c>
     </row>
     <row r="116" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>410</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
       <c r="M116">
         <v>117</v>
       </c>
@@ -15571,6 +15799,12 @@
       </c>
     </row>
     <row r="117" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>411</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
       <c r="M117">
         <v>118</v>
       </c>
@@ -15582,6 +15816,12 @@
       </c>
     </row>
     <row r="118" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>412</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
       <c r="M118">
         <v>119</v>
       </c>
@@ -15593,6 +15833,12 @@
       </c>
     </row>
     <row r="119" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
+        <v>413</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
       <c r="M119">
         <v>120</v>
       </c>
@@ -15604,6 +15850,12 @@
       </c>
     </row>
     <row r="120" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>414</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
       <c r="M120">
         <v>121</v>
       </c>
@@ -15615,6 +15867,12 @@
       </c>
     </row>
     <row r="121" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>415</v>
+      </c>
+      <c r="C121">
+        <v>0</v>
+      </c>
       <c r="M121">
         <v>122</v>
       </c>
@@ -15626,6 +15884,12 @@
       </c>
     </row>
     <row r="122" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
+        <v>416</v>
+      </c>
+      <c r="C122">
+        <v>0</v>
+      </c>
       <c r="M122">
         <v>123</v>
       </c>
@@ -15637,6 +15901,12 @@
       </c>
     </row>
     <row r="123" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
+        <v>417</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
       <c r="M123">
         <v>124</v>
       </c>
@@ -15645,6 +15915,238 @@
       </c>
       <c r="O123">
         <v>113</v>
+      </c>
+    </row>
+    <row r="124" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
+        <v>418</v>
+      </c>
+      <c r="C124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
+        <v>419</v>
+      </c>
+      <c r="C125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
+        <v>420</v>
+      </c>
+      <c r="C126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
+        <v>421</v>
+      </c>
+      <c r="C127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>422</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>423</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>424</v>
+      </c>
+      <c r="C130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>425</v>
+      </c>
+      <c r="C131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>426</v>
+      </c>
+      <c r="C132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>427</v>
+      </c>
+      <c r="C133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>428</v>
+      </c>
+      <c r="C134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>429</v>
+      </c>
+      <c r="C135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>430</v>
+      </c>
+      <c r="C136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>431</v>
+      </c>
+      <c r="C137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>432</v>
+      </c>
+      <c r="C138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>433</v>
+      </c>
+      <c r="C139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>434</v>
+      </c>
+      <c r="C140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>435</v>
+      </c>
+      <c r="C141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>436</v>
+      </c>
+      <c r="C142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>437</v>
+      </c>
+      <c r="C143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>438</v>
+      </c>
+      <c r="C144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>439</v>
+      </c>
+      <c r="C145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>440</v>
+      </c>
+      <c r="C146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>441</v>
+      </c>
+      <c r="C147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>442</v>
+      </c>
+      <c r="C148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
+        <v>443</v>
+      </c>
+      <c r="C149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>444</v>
+      </c>
+      <c r="C150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
+        <v>445</v>
+      </c>
+      <c r="C151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B152" t="s">
+        <v>446</v>
+      </c>
+      <c r="C152">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -15652,5 +16154,6 @@
     <sortCondition ref="K1:K133"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Configuration + classification changed
</commit_message>
<xml_diff>
--- a/DataBase/BreedCatsData.xlsx
+++ b/DataBase/BreedCatsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\source\repos\CatsCenter\DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067F792B-EF7B-44F7-9712-F60532DADDDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B061E87-30DD-4421-94CA-103A511B5E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F0E8892A-E61F-468D-BA28-553DFEA2DB6C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="496">
   <si>
     <r>
       <t>Abyssinian</t>
@@ -3315,12 +3315,6 @@
   </si>
   <si>
     <t>Cymric or Manx Longhair</t>
-  </si>
-  <si>
-    <t>Colorpoint Persian</t>
-  </si>
-  <si>
-    <t>Colorpoint Longhair</t>
   </si>
   <si>
     <t>Neva Masquerade (colorpoint Siberian)</t>
@@ -3969,14 +3963,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3987,6 +3981,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3994,15 +3997,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -10349,13 +10343,13 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="30" t="s">
         <v>39</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="33" t="s">
         <v>42</v>
       </c>
       <c r="D13" s="27" t="s">
@@ -10369,43 +10363,43 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="8"/>
-      <c r="C14" s="31"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
       <c r="F14" s="28"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="8"/>
-      <c r="C15" s="31"/>
+      <c r="C15" s="34"/>
       <c r="D15" s="28"/>
       <c r="E15" s="28"/>
       <c r="F15" s="28"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="31"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="9"/>
-      <c r="C17" s="31"/>
+      <c r="C17" s="34"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
     </row>
     <row r="18" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="26"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="32"/>
+      <c r="C18" s="35"/>
       <c r="D18" s="29"/>
       <c r="E18" s="29"/>
       <c r="F18" s="29"/>
@@ -10431,7 +10425,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="30" t="s">
         <v>50</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -10451,7 +10445,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
+      <c r="A21" s="31"/>
       <c r="B21" s="8"/>
       <c r="C21" s="28"/>
       <c r="D21" s="28"/>
@@ -10459,7 +10453,7 @@
       <c r="F21" s="28"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="9"/>
       <c r="C22" s="28"/>
       <c r="D22" s="28"/>
@@ -10467,7 +10461,7 @@
       <c r="F22" s="28"/>
     </row>
     <row r="23" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="26"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="10" t="s">
         <v>52</v>
       </c>
@@ -10477,7 +10471,7 @@
       <c r="F23" s="29"/>
     </row>
     <row r="24" spans="1:6" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="30" t="s">
         <v>56</v>
       </c>
       <c r="B24" s="11" t="s">
@@ -10497,7 +10491,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="8"/>
       <c r="C25" s="28"/>
       <c r="D25" s="28"/>
@@ -10505,7 +10499,7 @@
       <c r="F25" s="28"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
+      <c r="A26" s="31"/>
       <c r="B26" s="8"/>
       <c r="C26" s="28"/>
       <c r="D26" s="28"/>
@@ -10513,7 +10507,7 @@
       <c r="F26" s="28"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="25"/>
+      <c r="A27" s="31"/>
       <c r="B27" s="8"/>
       <c r="C27" s="28"/>
       <c r="D27" s="28"/>
@@ -10521,7 +10515,7 @@
       <c r="F27" s="28"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
+      <c r="A28" s="31"/>
       <c r="B28" s="8"/>
       <c r="C28" s="28"/>
       <c r="D28" s="28"/>
@@ -10529,7 +10523,7 @@
       <c r="F28" s="28"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
+      <c r="A29" s="31"/>
       <c r="B29" s="9"/>
       <c r="C29" s="28"/>
       <c r="D29" s="28"/>
@@ -10537,7 +10531,7 @@
       <c r="F29" s="28"/>
     </row>
     <row r="30" spans="1:6" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="26"/>
+      <c r="A30" s="32"/>
       <c r="B30" s="12" t="s">
         <v>58</v>
       </c>
@@ -10767,7 +10761,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="24" t="s">
+      <c r="A42" s="30" t="s">
         <v>95</v>
       </c>
       <c r="B42" s="11" t="s">
@@ -10787,7 +10781,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
+      <c r="A43" s="31"/>
       <c r="B43" s="8"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
@@ -10795,7 +10789,7 @@
       <c r="F43" s="28"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
+      <c r="A44" s="31"/>
       <c r="B44" s="8"/>
       <c r="C44" s="28"/>
       <c r="D44" s="28"/>
@@ -10803,7 +10797,7 @@
       <c r="F44" s="28"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="25"/>
+      <c r="A45" s="31"/>
       <c r="B45" s="8"/>
       <c r="C45" s="28"/>
       <c r="D45" s="28"/>
@@ -10811,7 +10805,7 @@
       <c r="F45" s="28"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="25"/>
+      <c r="A46" s="31"/>
       <c r="B46" s="8"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
@@ -10819,7 +10813,7 @@
       <c r="F46" s="28"/>
     </row>
     <row r="47" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="26"/>
+      <c r="A47" s="32"/>
       <c r="B47" s="10" t="s">
         <v>31</v>
       </c>
@@ -11125,7 +11119,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="85.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="24" t="s">
+      <c r="A68" s="30" t="s">
         <v>123</v>
       </c>
       <c r="B68" s="11" t="s">
@@ -11145,7 +11139,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="25"/>
+      <c r="A69" s="31"/>
       <c r="B69" s="8"/>
       <c r="C69" s="28"/>
       <c r="D69" s="28"/>
@@ -11153,7 +11147,7 @@
       <c r="F69" s="28"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="25"/>
+      <c r="A70" s="31"/>
       <c r="B70" s="8"/>
       <c r="C70" s="28"/>
       <c r="D70" s="28"/>
@@ -11161,7 +11155,7 @@
       <c r="F70" s="28"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="25"/>
+      <c r="A71" s="31"/>
       <c r="B71" s="9"/>
       <c r="C71" s="28"/>
       <c r="D71" s="28"/>
@@ -11169,7 +11163,7 @@
       <c r="F71" s="28"/>
     </row>
     <row r="72" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="26"/>
+      <c r="A72" s="32"/>
       <c r="B72" s="10" t="s">
         <v>41</v>
       </c>
@@ -11202,7 +11196,7 @@
       <c r="A74" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B74" s="30" t="s">
+      <c r="B74" s="33" t="s">
         <v>132</v>
       </c>
       <c r="C74" s="27" t="s">
@@ -11220,7 +11214,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="13"/>
-      <c r="B75" s="31"/>
+      <c r="B75" s="34"/>
       <c r="C75" s="28"/>
       <c r="D75" s="28"/>
       <c r="E75" s="28"/>
@@ -11228,7 +11222,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="13"/>
-      <c r="B76" s="31"/>
+      <c r="B76" s="34"/>
       <c r="C76" s="28"/>
       <c r="D76" s="28"/>
       <c r="E76" s="28"/>
@@ -11236,7 +11230,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="14"/>
-      <c r="B77" s="31"/>
+      <c r="B77" s="34"/>
       <c r="C77" s="28"/>
       <c r="D77" s="28"/>
       <c r="E77" s="28"/>
@@ -11246,7 +11240,7 @@
       <c r="A78" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="B78" s="32"/>
+      <c r="B78" s="35"/>
       <c r="C78" s="29"/>
       <c r="D78" s="29"/>
       <c r="E78" s="29"/>
@@ -11444,7 +11438,7 @@
       <c r="A90" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="B90" s="33" t="s">
+      <c r="B90" s="24" t="s">
         <v>163</v>
       </c>
       <c r="C90" s="27" t="s">
@@ -11453,7 +11447,7 @@
       <c r="D90" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="E90" s="30" t="s">
+      <c r="E90" s="33" t="s">
         <v>164</v>
       </c>
       <c r="F90" s="27" t="s">
@@ -11462,36 +11456,36 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="13"/>
-      <c r="B91" s="34"/>
+      <c r="B91" s="25"/>
       <c r="C91" s="28"/>
       <c r="D91" s="28"/>
-      <c r="E91" s="31"/>
+      <c r="E91" s="34"/>
       <c r="F91" s="28"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="13"/>
-      <c r="B92" s="34"/>
+      <c r="B92" s="25"/>
       <c r="C92" s="28"/>
       <c r="D92" s="28"/>
-      <c r="E92" s="31"/>
+      <c r="E92" s="34"/>
       <c r="F92" s="28"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="14"/>
-      <c r="B93" s="34"/>
+      <c r="B93" s="25"/>
       <c r="C93" s="28"/>
       <c r="D93" s="28"/>
-      <c r="E93" s="31"/>
+      <c r="E93" s="34"/>
       <c r="F93" s="28"/>
     </row>
     <row r="94" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="B94" s="35"/>
+      <c r="B94" s="26"/>
       <c r="C94" s="29"/>
       <c r="D94" s="29"/>
-      <c r="E94" s="32"/>
+      <c r="E94" s="35"/>
       <c r="F94" s="29"/>
     </row>
     <row r="95" spans="1:6" ht="114.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11595,7 +11589,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="24" t="s">
+      <c r="A100" s="30" t="s">
         <v>177</v>
       </c>
       <c r="B100" s="11" t="s">
@@ -11615,7 +11609,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="25"/>
+      <c r="A101" s="31"/>
       <c r="B101" s="8"/>
       <c r="C101" s="28"/>
       <c r="D101" s="28"/>
@@ -11623,7 +11617,7 @@
       <c r="F101" s="28"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="25"/>
+      <c r="A102" s="31"/>
       <c r="B102" s="9"/>
       <c r="C102" s="28"/>
       <c r="D102" s="28"/>
@@ -11631,7 +11625,7 @@
       <c r="F102" s="28"/>
     </row>
     <row r="103" spans="1:6" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="26"/>
+      <c r="A103" s="32"/>
       <c r="B103" s="10" t="s">
         <v>179</v>
       </c>
@@ -11875,7 +11869,7 @@
       <c r="F119" s="29"/>
     </row>
     <row r="120" spans="1:6" ht="171" x14ac:dyDescent="0.25">
-      <c r="A120" s="24" t="s">
+      <c r="A120" s="30" t="s">
         <v>202</v>
       </c>
       <c r="B120" s="11" t="s">
@@ -11895,7 +11889,7 @@
       </c>
     </row>
     <row r="121" spans="1:6" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="26"/>
+      <c r="A121" s="32"/>
       <c r="B121" s="10" t="s">
         <v>204</v>
       </c>
@@ -11920,7 +11914,7 @@
       <c r="E122" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="F122" s="30" t="s">
+      <c r="F122" s="33" t="s">
         <v>211</v>
       </c>
     </row>
@@ -11930,7 +11924,7 @@
       <c r="C123" s="28"/>
       <c r="D123" s="28"/>
       <c r="E123" s="28"/>
-      <c r="F123" s="31"/>
+      <c r="F123" s="34"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="37"/>
@@ -11938,7 +11932,7 @@
       <c r="C124" s="28"/>
       <c r="D124" s="28"/>
       <c r="E124" s="28"/>
-      <c r="F124" s="31"/>
+      <c r="F124" s="34"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="37"/>
@@ -11946,7 +11940,7 @@
       <c r="C125" s="28"/>
       <c r="D125" s="28"/>
       <c r="E125" s="28"/>
-      <c r="F125" s="31"/>
+      <c r="F125" s="34"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="37"/>
@@ -11954,7 +11948,7 @@
       <c r="C126" s="28"/>
       <c r="D126" s="28"/>
       <c r="E126" s="28"/>
-      <c r="F126" s="31"/>
+      <c r="F126" s="34"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="37"/>
@@ -11962,7 +11956,7 @@
       <c r="C127" s="28"/>
       <c r="D127" s="28"/>
       <c r="E127" s="28"/>
-      <c r="F127" s="31"/>
+      <c r="F127" s="34"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="37"/>
@@ -11970,7 +11964,7 @@
       <c r="C128" s="28"/>
       <c r="D128" s="28"/>
       <c r="E128" s="28"/>
-      <c r="F128" s="31"/>
+      <c r="F128" s="34"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="37"/>
@@ -11978,7 +11972,7 @@
       <c r="C129" s="28"/>
       <c r="D129" s="28"/>
       <c r="E129" s="28"/>
-      <c r="F129" s="31"/>
+      <c r="F129" s="34"/>
     </row>
     <row r="130" spans="1:6" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="38"/>
@@ -11988,7 +11982,7 @@
       <c r="C130" s="29"/>
       <c r="D130" s="29"/>
       <c r="E130" s="29"/>
-      <c r="F130" s="32"/>
+      <c r="F130" s="35"/>
     </row>
     <row r="131" spans="1:6" ht="114" x14ac:dyDescent="0.25">
       <c r="A131" s="36" t="s">
@@ -12093,7 +12087,7 @@
       <c r="F141" s="29"/>
     </row>
     <row r="142" spans="1:6" ht="85.5" x14ac:dyDescent="0.25">
-      <c r="A142" s="24" t="s">
+      <c r="A142" s="30" t="s">
         <v>214</v>
       </c>
       <c r="B142" s="11" t="s">
@@ -12113,7 +12107,7 @@
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A143" s="25"/>
+      <c r="A143" s="31"/>
       <c r="B143" s="8"/>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -12121,7 +12115,7 @@
       <c r="F143" s="28"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A144" s="25"/>
+      <c r="A144" s="31"/>
       <c r="B144" s="8"/>
       <c r="C144" s="28"/>
       <c r="D144" s="28"/>
@@ -12129,7 +12123,7 @@
       <c r="F144" s="28"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A145" s="25"/>
+      <c r="A145" s="31"/>
       <c r="B145" s="9"/>
       <c r="C145" s="28"/>
       <c r="D145" s="28"/>
@@ -12137,7 +12131,7 @@
       <c r="F145" s="28"/>
     </row>
     <row r="146" spans="1:6" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="26"/>
+      <c r="A146" s="32"/>
       <c r="B146" s="10" t="s">
         <v>216</v>
       </c>
@@ -12167,7 +12161,7 @@
       </c>
     </row>
     <row r="148" spans="1:6" ht="128.25" x14ac:dyDescent="0.25">
-      <c r="A148" s="24" t="s">
+      <c r="A148" s="30" t="s">
         <v>222</v>
       </c>
       <c r="B148" s="27" t="s">
@@ -12187,7 +12181,7 @@
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" s="25"/>
+      <c r="A149" s="31"/>
       <c r="B149" s="28"/>
       <c r="C149" s="8"/>
       <c r="D149" s="28"/>
@@ -12195,7 +12189,7 @@
       <c r="F149" s="28"/>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A150" s="25"/>
+      <c r="A150" s="31"/>
       <c r="B150" s="28"/>
       <c r="C150" s="8"/>
       <c r="D150" s="28"/>
@@ -12203,7 +12197,7 @@
       <c r="F150" s="28"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A151" s="25"/>
+      <c r="A151" s="31"/>
       <c r="B151" s="28"/>
       <c r="C151" s="8"/>
       <c r="D151" s="28"/>
@@ -12211,7 +12205,7 @@
       <c r="F151" s="28"/>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A152" s="25"/>
+      <c r="A152" s="31"/>
       <c r="B152" s="28"/>
       <c r="C152" s="8"/>
       <c r="D152" s="28"/>
@@ -12219,7 +12213,7 @@
       <c r="F152" s="28"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A153" s="25"/>
+      <c r="A153" s="31"/>
       <c r="B153" s="28"/>
       <c r="C153" s="9"/>
       <c r="D153" s="28"/>
@@ -12227,7 +12221,7 @@
       <c r="F153" s="28"/>
     </row>
     <row r="154" spans="1:6" ht="114.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="26"/>
+      <c r="A154" s="32"/>
       <c r="B154" s="29"/>
       <c r="C154" s="10" t="s">
         <v>224</v>
@@ -12363,7 +12357,7 @@
       </c>
     </row>
     <row r="163" spans="1:6" ht="57" x14ac:dyDescent="0.25">
-      <c r="A163" s="24" t="s">
+      <c r="A163" s="30" t="s">
         <v>241</v>
       </c>
       <c r="B163" s="11" t="s">
@@ -12383,7 +12377,7 @@
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A164" s="25"/>
+      <c r="A164" s="31"/>
       <c r="B164" s="8"/>
       <c r="C164" s="28"/>
       <c r="D164" s="28"/>
@@ -12391,7 +12385,7 @@
       <c r="F164" s="28"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A165" s="25"/>
+      <c r="A165" s="31"/>
       <c r="B165" s="8"/>
       <c r="C165" s="28"/>
       <c r="D165" s="28"/>
@@ -12399,7 +12393,7 @@
       <c r="F165" s="28"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A166" s="25"/>
+      <c r="A166" s="31"/>
       <c r="B166" s="8"/>
       <c r="C166" s="28"/>
       <c r="D166" s="28"/>
@@ -12407,7 +12401,7 @@
       <c r="F166" s="28"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A167" s="25"/>
+      <c r="A167" s="31"/>
       <c r="B167" s="8"/>
       <c r="C167" s="28"/>
       <c r="D167" s="28"/>
@@ -12415,7 +12409,7 @@
       <c r="F167" s="28"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A168" s="25"/>
+      <c r="A168" s="31"/>
       <c r="B168" s="8"/>
       <c r="C168" s="28"/>
       <c r="D168" s="28"/>
@@ -12423,7 +12417,7 @@
       <c r="F168" s="28"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A169" s="25"/>
+      <c r="A169" s="31"/>
       <c r="B169" s="9"/>
       <c r="C169" s="28"/>
       <c r="D169" s="28"/>
@@ -12431,7 +12425,7 @@
       <c r="F169" s="28"/>
     </row>
     <row r="170" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="26"/>
+      <c r="A170" s="32"/>
       <c r="B170" s="10" t="s">
         <v>243</v>
       </c>
@@ -12567,7 +12561,7 @@
       <c r="B177" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="C177" s="30" t="s">
+      <c r="C177" s="33" t="s">
         <v>267</v>
       </c>
       <c r="D177" s="27" t="s">
@@ -12585,7 +12579,7 @@
       <c r="B178" s="20" t="s">
         <v>266</v>
       </c>
-      <c r="C178" s="31"/>
+      <c r="C178" s="34"/>
       <c r="D178" s="28"/>
       <c r="E178" s="28"/>
       <c r="F178" s="28"/>
@@ -12593,7 +12587,7 @@
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="13"/>
       <c r="B179" s="9"/>
-      <c r="C179" s="31"/>
+      <c r="C179" s="34"/>
       <c r="D179" s="28"/>
       <c r="E179" s="28"/>
       <c r="F179" s="28"/>
@@ -12601,7 +12595,7 @@
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="13"/>
       <c r="B180" s="9"/>
-      <c r="C180" s="31"/>
+      <c r="C180" s="34"/>
       <c r="D180" s="28"/>
       <c r="E180" s="28"/>
       <c r="F180" s="28"/>
@@ -12611,7 +12605,7 @@
         <v>265</v>
       </c>
       <c r="B181" s="10"/>
-      <c r="C181" s="32"/>
+      <c r="C181" s="35"/>
       <c r="D181" s="29"/>
       <c r="E181" s="29"/>
       <c r="F181" s="29"/>
@@ -12620,90 +12614,90 @@
       <c r="A182" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="B182" s="30" t="s">
+      <c r="B182" s="33" t="s">
         <v>271</v>
       </c>
       <c r="C182" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D182" s="30" t="s">
+      <c r="D182" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="E182" s="30" t="s">
+      <c r="E182" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="F182" s="30" t="s">
+      <c r="F182" s="33" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="13"/>
-      <c r="B183" s="31"/>
+      <c r="B183" s="34"/>
       <c r="C183" s="28"/>
-      <c r="D183" s="31"/>
-      <c r="E183" s="31"/>
-      <c r="F183" s="31"/>
+      <c r="D183" s="34"/>
+      <c r="E183" s="34"/>
+      <c r="F183" s="34"/>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="13"/>
-      <c r="B184" s="31"/>
+      <c r="B184" s="34"/>
       <c r="C184" s="28"/>
-      <c r="D184" s="31"/>
-      <c r="E184" s="31"/>
-      <c r="F184" s="31"/>
+      <c r="D184" s="34"/>
+      <c r="E184" s="34"/>
+      <c r="F184" s="34"/>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="13"/>
-      <c r="B185" s="31"/>
+      <c r="B185" s="34"/>
       <c r="C185" s="28"/>
-      <c r="D185" s="31"/>
-      <c r="E185" s="31"/>
-      <c r="F185" s="31"/>
+      <c r="D185" s="34"/>
+      <c r="E185" s="34"/>
+      <c r="F185" s="34"/>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="13"/>
-      <c r="B186" s="31"/>
+      <c r="B186" s="34"/>
       <c r="C186" s="28"/>
-      <c r="D186" s="31"/>
-      <c r="E186" s="31"/>
-      <c r="F186" s="31"/>
+      <c r="D186" s="34"/>
+      <c r="E186" s="34"/>
+      <c r="F186" s="34"/>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="13"/>
-      <c r="B187" s="31"/>
+      <c r="B187" s="34"/>
       <c r="C187" s="28"/>
-      <c r="D187" s="31"/>
-      <c r="E187" s="31"/>
-      <c r="F187" s="31"/>
+      <c r="D187" s="34"/>
+      <c r="E187" s="34"/>
+      <c r="F187" s="34"/>
     </row>
     <row r="188" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A188" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="B188" s="31"/>
+      <c r="B188" s="34"/>
       <c r="C188" s="28"/>
-      <c r="D188" s="31"/>
-      <c r="E188" s="31"/>
-      <c r="F188" s="31"/>
+      <c r="D188" s="34"/>
+      <c r="E188" s="34"/>
+      <c r="F188" s="34"/>
     </row>
     <row r="189" spans="1:6" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="B189" s="32"/>
+      <c r="B189" s="35"/>
       <c r="C189" s="29"/>
-      <c r="D189" s="32"/>
-      <c r="E189" s="32"/>
-      <c r="F189" s="32"/>
+      <c r="D189" s="35"/>
+      <c r="E189" s="35"/>
+      <c r="F189" s="35"/>
     </row>
     <row r="190" spans="1:6" ht="57" x14ac:dyDescent="0.25">
-      <c r="A190" s="24" t="s">
+      <c r="A190" s="30" t="s">
         <v>273</v>
       </c>
       <c r="B190" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="C190" s="30" t="s">
+      <c r="C190" s="33" t="s">
         <v>276</v>
       </c>
       <c r="D190" s="27" t="s">
@@ -12717,59 +12711,59 @@
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A191" s="25"/>
+      <c r="A191" s="31"/>
       <c r="B191" s="8"/>
-      <c r="C191" s="31"/>
+      <c r="C191" s="34"/>
       <c r="D191" s="28"/>
       <c r="E191" s="28"/>
       <c r="F191" s="28"/>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A192" s="25"/>
+      <c r="A192" s="31"/>
       <c r="B192" s="8"/>
-      <c r="C192" s="31"/>
+      <c r="C192" s="34"/>
       <c r="D192" s="28"/>
       <c r="E192" s="28"/>
       <c r="F192" s="28"/>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A193" s="25"/>
+      <c r="A193" s="31"/>
       <c r="B193" s="8"/>
-      <c r="C193" s="31"/>
+      <c r="C193" s="34"/>
       <c r="D193" s="28"/>
       <c r="E193" s="28"/>
       <c r="F193" s="28"/>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A194" s="25"/>
+      <c r="A194" s="31"/>
       <c r="B194" s="8"/>
-      <c r="C194" s="31"/>
+      <c r="C194" s="34"/>
       <c r="D194" s="28"/>
       <c r="E194" s="28"/>
       <c r="F194" s="28"/>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A195" s="25"/>
+      <c r="A195" s="31"/>
       <c r="B195" s="8"/>
-      <c r="C195" s="31"/>
+      <c r="C195" s="34"/>
       <c r="D195" s="28"/>
       <c r="E195" s="28"/>
       <c r="F195" s="28"/>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A196" s="25"/>
+      <c r="A196" s="31"/>
       <c r="B196" s="9"/>
-      <c r="C196" s="31"/>
+      <c r="C196" s="34"/>
       <c r="D196" s="28"/>
       <c r="E196" s="28"/>
       <c r="F196" s="28"/>
     </row>
     <row r="197" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A197" s="26"/>
+      <c r="A197" s="32"/>
       <c r="B197" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="C197" s="32"/>
+      <c r="C197" s="35"/>
       <c r="D197" s="29"/>
       <c r="E197" s="29"/>
       <c r="F197" s="29"/>
@@ -13065,7 +13059,7 @@
       </c>
     </row>
     <row r="217" spans="1:6" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="A217" s="24" t="s">
+      <c r="A217" s="30" t="s">
         <v>304</v>
       </c>
       <c r="B217" s="11" t="s">
@@ -13085,7 +13079,7 @@
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A218" s="25"/>
+      <c r="A218" s="31"/>
       <c r="B218" s="8"/>
       <c r="C218" s="28"/>
       <c r="D218" s="28"/>
@@ -13093,7 +13087,7 @@
       <c r="F218" s="28"/>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A219" s="25"/>
+      <c r="A219" s="31"/>
       <c r="B219" s="8"/>
       <c r="C219" s="28"/>
       <c r="D219" s="28"/>
@@ -13101,7 +13095,7 @@
       <c r="F219" s="28"/>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A220" s="25"/>
+      <c r="A220" s="31"/>
       <c r="B220" s="8"/>
       <c r="C220" s="28"/>
       <c r="D220" s="28"/>
@@ -13109,7 +13103,7 @@
       <c r="F220" s="28"/>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A221" s="25"/>
+      <c r="A221" s="31"/>
       <c r="B221" s="9"/>
       <c r="C221" s="28"/>
       <c r="D221" s="28"/>
@@ -13117,7 +13111,7 @@
       <c r="F221" s="28"/>
     </row>
     <row r="222" spans="1:6" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A222" s="26"/>
+      <c r="A222" s="32"/>
       <c r="B222" s="10" t="s">
         <v>306</v>
       </c>
@@ -13130,7 +13124,7 @@
       <c r="A223" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="B223" s="33" t="s">
+      <c r="B223" s="24" t="s">
         <v>310</v>
       </c>
       <c r="C223" s="27" t="s">
@@ -13148,7 +13142,7 @@
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="13"/>
-      <c r="B224" s="34"/>
+      <c r="B224" s="25"/>
       <c r="C224" s="28"/>
       <c r="D224" s="28"/>
       <c r="E224" s="28"/>
@@ -13156,7 +13150,7 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="13"/>
-      <c r="B225" s="34"/>
+      <c r="B225" s="25"/>
       <c r="C225" s="28"/>
       <c r="D225" s="28"/>
       <c r="E225" s="28"/>
@@ -13164,7 +13158,7 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="18"/>
-      <c r="B226" s="34"/>
+      <c r="B226" s="25"/>
       <c r="C226" s="28"/>
       <c r="D226" s="28"/>
       <c r="E226" s="28"/>
@@ -13174,7 +13168,7 @@
       <c r="A227" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="B227" s="35"/>
+      <c r="B227" s="26"/>
       <c r="C227" s="29"/>
       <c r="D227" s="29"/>
       <c r="E227" s="29"/>
@@ -13222,74 +13216,46 @@
     </row>
   </sheetData>
   <mergeCells count="122">
-    <mergeCell ref="B223:B227"/>
-    <mergeCell ref="C223:C227"/>
-    <mergeCell ref="D223:D227"/>
-    <mergeCell ref="E223:E227"/>
-    <mergeCell ref="F223:F227"/>
-    <mergeCell ref="C203:C211"/>
-    <mergeCell ref="D203:D211"/>
-    <mergeCell ref="E203:E211"/>
-    <mergeCell ref="F203:F211"/>
-    <mergeCell ref="A217:A222"/>
-    <mergeCell ref="C217:C222"/>
-    <mergeCell ref="D217:D222"/>
-    <mergeCell ref="E217:E222"/>
-    <mergeCell ref="F217:F222"/>
-    <mergeCell ref="A190:A197"/>
-    <mergeCell ref="C190:C197"/>
-    <mergeCell ref="D190:D197"/>
-    <mergeCell ref="E190:E197"/>
-    <mergeCell ref="F190:F197"/>
-    <mergeCell ref="C177:C181"/>
-    <mergeCell ref="D177:D181"/>
-    <mergeCell ref="E177:E181"/>
-    <mergeCell ref="F177:F181"/>
-    <mergeCell ref="B182:B189"/>
-    <mergeCell ref="C182:C189"/>
-    <mergeCell ref="D182:D189"/>
-    <mergeCell ref="E182:E189"/>
-    <mergeCell ref="F182:F189"/>
-    <mergeCell ref="A163:A170"/>
-    <mergeCell ref="C163:C170"/>
-    <mergeCell ref="D163:D170"/>
-    <mergeCell ref="E163:E170"/>
-    <mergeCell ref="F163:F170"/>
-    <mergeCell ref="B156:B159"/>
-    <mergeCell ref="C156:C159"/>
-    <mergeCell ref="D156:D159"/>
-    <mergeCell ref="E156:E159"/>
-    <mergeCell ref="F156:F159"/>
-    <mergeCell ref="A148:A154"/>
-    <mergeCell ref="B148:B154"/>
-    <mergeCell ref="D148:D154"/>
-    <mergeCell ref="E148:E154"/>
-    <mergeCell ref="F148:F154"/>
-    <mergeCell ref="A142:A146"/>
-    <mergeCell ref="C142:C146"/>
-    <mergeCell ref="D142:D146"/>
-    <mergeCell ref="E142:E146"/>
-    <mergeCell ref="F142:F146"/>
-    <mergeCell ref="A131:A141"/>
-    <mergeCell ref="C131:C141"/>
-    <mergeCell ref="D131:D141"/>
-    <mergeCell ref="E131:E141"/>
-    <mergeCell ref="F131:F141"/>
-    <mergeCell ref="A122:A130"/>
-    <mergeCell ref="C122:C130"/>
-    <mergeCell ref="D122:D130"/>
-    <mergeCell ref="E122:E130"/>
-    <mergeCell ref="F122:F130"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="C120:C121"/>
-    <mergeCell ref="D120:D121"/>
-    <mergeCell ref="E120:E121"/>
-    <mergeCell ref="F120:F121"/>
-    <mergeCell ref="B112:B119"/>
-    <mergeCell ref="C112:C119"/>
-    <mergeCell ref="D112:D119"/>
-    <mergeCell ref="E112:E119"/>
-    <mergeCell ref="F112:F119"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="A13:A18"/>
+    <mergeCell ref="C13:C18"/>
+    <mergeCell ref="D13:D18"/>
+    <mergeCell ref="E13:E18"/>
+    <mergeCell ref="F13:F18"/>
+    <mergeCell ref="A42:A47"/>
+    <mergeCell ref="C42:C47"/>
+    <mergeCell ref="D42:D47"/>
+    <mergeCell ref="E42:E47"/>
+    <mergeCell ref="F42:F47"/>
+    <mergeCell ref="A24:A30"/>
+    <mergeCell ref="C24:C30"/>
+    <mergeCell ref="D24:D30"/>
+    <mergeCell ref="E24:E30"/>
+    <mergeCell ref="F24:F30"/>
+    <mergeCell ref="B56:B61"/>
+    <mergeCell ref="C56:C61"/>
+    <mergeCell ref="D56:D61"/>
+    <mergeCell ref="E56:E61"/>
+    <mergeCell ref="F56:F61"/>
+    <mergeCell ref="B51:B55"/>
+    <mergeCell ref="C51:C55"/>
+    <mergeCell ref="D51:D55"/>
+    <mergeCell ref="E51:E55"/>
+    <mergeCell ref="F51:F55"/>
+    <mergeCell ref="B74:B78"/>
+    <mergeCell ref="C74:C78"/>
+    <mergeCell ref="D74:D78"/>
+    <mergeCell ref="E74:E78"/>
+    <mergeCell ref="F74:F78"/>
+    <mergeCell ref="A68:A72"/>
+    <mergeCell ref="C68:C72"/>
+    <mergeCell ref="D68:D72"/>
+    <mergeCell ref="E68:E72"/>
+    <mergeCell ref="F68:F72"/>
     <mergeCell ref="A100:A103"/>
     <mergeCell ref="C100:C103"/>
     <mergeCell ref="D100:D103"/>
@@ -13304,46 +13270,74 @@
     <mergeCell ref="D90:D94"/>
     <mergeCell ref="E90:E94"/>
     <mergeCell ref="F90:F94"/>
-    <mergeCell ref="B74:B78"/>
-    <mergeCell ref="C74:C78"/>
-    <mergeCell ref="D74:D78"/>
-    <mergeCell ref="E74:E78"/>
-    <mergeCell ref="F74:F78"/>
-    <mergeCell ref="A68:A72"/>
-    <mergeCell ref="C68:C72"/>
-    <mergeCell ref="D68:D72"/>
-    <mergeCell ref="E68:E72"/>
-    <mergeCell ref="F68:F72"/>
-    <mergeCell ref="B56:B61"/>
-    <mergeCell ref="C56:C61"/>
-    <mergeCell ref="D56:D61"/>
-    <mergeCell ref="E56:E61"/>
-    <mergeCell ref="F56:F61"/>
-    <mergeCell ref="B51:B55"/>
-    <mergeCell ref="C51:C55"/>
-    <mergeCell ref="D51:D55"/>
-    <mergeCell ref="E51:E55"/>
-    <mergeCell ref="F51:F55"/>
-    <mergeCell ref="A42:A47"/>
-    <mergeCell ref="C42:C47"/>
-    <mergeCell ref="D42:D47"/>
-    <mergeCell ref="E42:E47"/>
-    <mergeCell ref="F42:F47"/>
-    <mergeCell ref="A24:A30"/>
-    <mergeCell ref="C24:C30"/>
-    <mergeCell ref="D24:D30"/>
-    <mergeCell ref="E24:E30"/>
-    <mergeCell ref="F24:F30"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="C13:C18"/>
-    <mergeCell ref="D13:D18"/>
-    <mergeCell ref="E13:E18"/>
-    <mergeCell ref="F13:F18"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="C120:C121"/>
+    <mergeCell ref="D120:D121"/>
+    <mergeCell ref="E120:E121"/>
+    <mergeCell ref="F120:F121"/>
+    <mergeCell ref="B112:B119"/>
+    <mergeCell ref="C112:C119"/>
+    <mergeCell ref="D112:D119"/>
+    <mergeCell ref="E112:E119"/>
+    <mergeCell ref="F112:F119"/>
+    <mergeCell ref="A131:A141"/>
+    <mergeCell ref="C131:C141"/>
+    <mergeCell ref="D131:D141"/>
+    <mergeCell ref="E131:E141"/>
+    <mergeCell ref="F131:F141"/>
+    <mergeCell ref="A122:A130"/>
+    <mergeCell ref="C122:C130"/>
+    <mergeCell ref="D122:D130"/>
+    <mergeCell ref="E122:E130"/>
+    <mergeCell ref="F122:F130"/>
+    <mergeCell ref="A148:A154"/>
+    <mergeCell ref="B148:B154"/>
+    <mergeCell ref="D148:D154"/>
+    <mergeCell ref="E148:E154"/>
+    <mergeCell ref="F148:F154"/>
+    <mergeCell ref="A142:A146"/>
+    <mergeCell ref="C142:C146"/>
+    <mergeCell ref="D142:D146"/>
+    <mergeCell ref="E142:E146"/>
+    <mergeCell ref="F142:F146"/>
+    <mergeCell ref="A163:A170"/>
+    <mergeCell ref="C163:C170"/>
+    <mergeCell ref="D163:D170"/>
+    <mergeCell ref="E163:E170"/>
+    <mergeCell ref="F163:F170"/>
+    <mergeCell ref="B156:B159"/>
+    <mergeCell ref="C156:C159"/>
+    <mergeCell ref="D156:D159"/>
+    <mergeCell ref="E156:E159"/>
+    <mergeCell ref="F156:F159"/>
+    <mergeCell ref="C177:C181"/>
+    <mergeCell ref="D177:D181"/>
+    <mergeCell ref="E177:E181"/>
+    <mergeCell ref="F177:F181"/>
+    <mergeCell ref="B182:B189"/>
+    <mergeCell ref="C182:C189"/>
+    <mergeCell ref="D182:D189"/>
+    <mergeCell ref="E182:E189"/>
+    <mergeCell ref="F182:F189"/>
+    <mergeCell ref="A217:A222"/>
+    <mergeCell ref="C217:C222"/>
+    <mergeCell ref="D217:D222"/>
+    <mergeCell ref="E217:E222"/>
+    <mergeCell ref="F217:F222"/>
+    <mergeCell ref="A190:A197"/>
+    <mergeCell ref="C190:C197"/>
+    <mergeCell ref="D190:D197"/>
+    <mergeCell ref="E190:E197"/>
+    <mergeCell ref="F190:F197"/>
+    <mergeCell ref="B223:B227"/>
+    <mergeCell ref="C223:C227"/>
+    <mergeCell ref="D223:D227"/>
+    <mergeCell ref="E223:E227"/>
+    <mergeCell ref="F223:F227"/>
+    <mergeCell ref="C203:C211"/>
+    <mergeCell ref="D203:D211"/>
+    <mergeCell ref="E203:E211"/>
+    <mergeCell ref="F203:F211"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" tooltip="Aegean cat" display="https://en.wikipedia.org/wiki/Aegean_cat" xr:uid="{6703FBD1-88B6-4565-9001-B3C67A67739E}"/>
@@ -13537,8 +13531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E730C0B2-6DE9-4F50-AD37-39852B7F947B}">
   <dimension ref="B1:S153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13576,13 +13570,13 @@
         <v>15</v>
       </c>
       <c r="M1" t="s">
+        <v>376</v>
+      </c>
+      <c r="N1" t="s">
+        <v>377</v>
+      </c>
+      <c r="O1" t="s">
         <v>378</v>
-      </c>
-      <c r="N1" t="s">
-        <v>379</v>
-      </c>
-      <c r="O1" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
@@ -13776,7 +13770,7 @@
         <v>362</v>
       </c>
       <c r="K8" s="21" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="M8">
         <v>7</v>
@@ -13818,12 +13812,6 @@
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
       <c r="E10" s="22" t="s">
         <v>351</v>
       </c>
@@ -13834,7 +13822,7 @@
         <v>169</v>
       </c>
       <c r="K10" s="21" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M10">
         <v>9</v>
@@ -13847,12 +13835,6 @@
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
       <c r="E11" s="22" t="s">
         <v>25</v>
       </c>
@@ -13860,7 +13842,7 @@
         <v>334</v>
       </c>
       <c r="K11" s="21" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M11">
         <v>10</v>
@@ -13886,7 +13868,7 @@
         <v>141</v>
       </c>
       <c r="K12" s="21" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="M12">
         <v>11</v>
@@ -13912,7 +13894,7 @@
         <v>160</v>
       </c>
       <c r="K13" s="21" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="M13">
         <v>12</v>
@@ -13938,7 +13920,7 @@
         <v>228</v>
       </c>
       <c r="K14" s="21" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="M14">
         <v>13</v>
@@ -13961,10 +13943,10 @@
         <v>262</v>
       </c>
       <c r="G15" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="K15" s="21" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M15">
         <v>14</v>
@@ -13987,7 +13969,7 @@
         <v>360</v>
       </c>
       <c r="K16" s="21" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="M16">
         <v>15</v>
@@ -14033,7 +14015,7 @@
         <v>7</v>
       </c>
       <c r="K18" s="21" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="M18">
         <v>17</v>
@@ -14079,7 +14061,7 @@
         <v>343</v>
       </c>
       <c r="K20" s="21" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="M20">
         <v>19</v>
@@ -14102,7 +14084,7 @@
         <v>345</v>
       </c>
       <c r="K21" s="21" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="M21">
         <v>20</v>
@@ -14194,7 +14176,7 @@
         <v>348</v>
       </c>
       <c r="K25" s="21" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="M25">
         <v>24</v>
@@ -14217,7 +14199,7 @@
         <v>346</v>
       </c>
       <c r="K26" s="21" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="M26">
         <v>25</v>
@@ -14240,7 +14222,7 @@
         <v>355</v>
       </c>
       <c r="K27" s="21" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="M27">
         <v>26</v>
@@ -14332,7 +14314,7 @@
         <v>342</v>
       </c>
       <c r="K31" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="M31">
         <v>30</v>
@@ -14346,7 +14328,7 @@
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -14378,7 +14360,7 @@
         <v>28</v>
       </c>
       <c r="K33" s="21" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="M33">
         <v>32</v>
@@ -14392,7 +14374,7 @@
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -14401,7 +14383,7 @@
         <v>338</v>
       </c>
       <c r="K34" s="23" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="M34">
         <v>33</v>
@@ -14414,12 +14396,6 @@
       </c>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>108</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
       <c r="E35" s="22" t="s">
         <v>31</v>
       </c>
@@ -14447,7 +14423,7 @@
         <v>83</v>
       </c>
       <c r="K36" s="23" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="M36">
         <v>35</v>
@@ -14493,7 +14469,7 @@
         <v>313</v>
       </c>
       <c r="K38" s="21" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="M38">
         <v>37</v>
@@ -14513,10 +14489,10 @@
         <v>1</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="K39" s="21" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="M39">
         <v>38</v>
@@ -14536,7 +14512,7 @@
         <v>1</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="K40" s="21" t="s">
         <v>148</v>
@@ -14559,10 +14535,10 @@
         <v>1</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="K41" s="21" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="M41">
         <v>40</v>
@@ -14582,7 +14558,7 @@
         <v>1</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="K42" s="21" t="s">
         <v>250</v>
@@ -14605,10 +14581,10 @@
         <v>1</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="K43" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="M43">
         <v>42</v>
@@ -14622,13 +14598,13 @@
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="K44" s="21" t="s">
         <v>81</v>
@@ -14644,17 +14620,11 @@
       </c>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>365</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
       <c r="E45" s="22" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="K45" s="21" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="M45">
         <v>44</v>
@@ -14688,7 +14658,7 @@
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -14707,12 +14677,6 @@
       </c>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>366</v>
-      </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
       <c r="K48" s="21" t="s">
         <v>307</v>
       </c>
@@ -14754,7 +14718,7 @@
         <v>1</v>
       </c>
       <c r="K50" s="21" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="M50">
         <v>49</v>
@@ -14766,10 +14730,10 @@
         <v>43</v>
       </c>
       <c r="R50" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="S50" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="51" spans="2:19" x14ac:dyDescent="0.25">
@@ -14780,7 +14744,7 @@
         <v>1</v>
       </c>
       <c r="K51" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="M51">
         <v>50</v>
@@ -14800,7 +14764,7 @@
         <v>1</v>
       </c>
       <c r="K52" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="M52">
         <v>51</v>
@@ -14820,7 +14784,7 @@
         <v>1</v>
       </c>
       <c r="K53" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="M53">
         <v>52</v>
@@ -14840,7 +14804,7 @@
         <v>1</v>
       </c>
       <c r="K54" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="M54">
         <v>53</v>
@@ -14854,13 +14818,13 @@
     </row>
     <row r="55" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
       <c r="K55" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="M55">
         <v>54</v>
@@ -14877,7 +14841,7 @@
         <v>1</v>
       </c>
       <c r="K56" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="M56">
         <v>55</v>
@@ -14897,7 +14861,7 @@
         <v>1</v>
       </c>
       <c r="K57" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="M57">
         <v>56</v>
@@ -14917,7 +14881,7 @@
         <v>1</v>
       </c>
       <c r="K58" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="M58">
         <v>57</v>
@@ -14937,7 +14901,7 @@
         <v>1</v>
       </c>
       <c r="K59" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="M59">
         <v>58</v>
@@ -14957,7 +14921,7 @@
         <v>1</v>
       </c>
       <c r="K60" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="M60">
         <v>59</v>
@@ -14977,7 +14941,7 @@
         <v>1</v>
       </c>
       <c r="K61" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="M61">
         <v>60</v>
@@ -14997,7 +14961,7 @@
         <v>1</v>
       </c>
       <c r="K62" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="M62">
         <v>61</v>
@@ -15017,7 +14981,7 @@
         <v>1</v>
       </c>
       <c r="K63" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="M63">
         <v>62</v>
@@ -15037,7 +15001,7 @@
         <v>1</v>
       </c>
       <c r="K64" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="M64">
         <v>63</v>
@@ -15057,7 +15021,7 @@
         <v>1</v>
       </c>
       <c r="K65" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="M65">
         <v>64</v>
@@ -15077,7 +15041,7 @@
         <v>1</v>
       </c>
       <c r="K66" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="M66">
         <v>65</v>
@@ -15091,13 +15055,13 @@
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
       <c r="K67" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="M67">
         <v>67</v>
@@ -15117,7 +15081,7 @@
         <v>1</v>
       </c>
       <c r="K68" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="M68">
         <v>68</v>
@@ -15137,7 +15101,7 @@
         <v>1</v>
       </c>
       <c r="K69" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="M69">
         <v>69</v>
@@ -15157,7 +15121,7 @@
         <v>1</v>
       </c>
       <c r="K70" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="M70">
         <v>70</v>
@@ -15177,7 +15141,7 @@
         <v>1</v>
       </c>
       <c r="K71" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="M71">
         <v>71</v>
@@ -15197,7 +15161,7 @@
         <v>1</v>
       </c>
       <c r="K72" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="M72">
         <v>72</v>
@@ -15211,7 +15175,7 @@
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K73" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="M73">
         <v>73</v>
@@ -15225,7 +15189,7 @@
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K74" s="23" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="M74">
         <v>74</v>
@@ -15245,7 +15209,7 @@
         <v>1</v>
       </c>
       <c r="K75" s="23" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="M75">
         <v>75</v>
@@ -15265,7 +15229,7 @@
         <v>1</v>
       </c>
       <c r="K76" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="M76">
         <v>76</v>
@@ -15285,7 +15249,7 @@
         <v>1</v>
       </c>
       <c r="K77" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="M77">
         <v>77</v>
@@ -15305,7 +15269,7 @@
         <v>1</v>
       </c>
       <c r="K78" s="23" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="M78">
         <v>78</v>
@@ -15325,7 +15289,7 @@
         <v>1</v>
       </c>
       <c r="K79" s="23" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="M79">
         <v>79</v>
@@ -15345,7 +15309,7 @@
         <v>1</v>
       </c>
       <c r="K80" s="23" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="M80">
         <v>80</v>
@@ -15365,7 +15329,7 @@
         <v>1</v>
       </c>
       <c r="K81" s="23" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="M81">
         <v>81</v>
@@ -15385,7 +15349,7 @@
         <v>1</v>
       </c>
       <c r="K82" s="23" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="M82">
         <v>82</v>
@@ -15405,7 +15369,7 @@
         <v>1</v>
       </c>
       <c r="K83" s="23" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="M83">
         <v>83</v>
@@ -15419,13 +15383,13 @@
     </row>
     <row r="84" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C84">
         <v>1</v>
       </c>
       <c r="K84" s="23" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="M84">
         <v>84</v>
@@ -15439,13 +15403,13 @@
     </row>
     <row r="85" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C85">
         <v>1</v>
       </c>
       <c r="K85" s="23" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="M85">
         <v>85</v>
@@ -15459,13 +15423,13 @@
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C86">
         <v>1</v>
       </c>
       <c r="K86" s="23" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="M86">
         <v>86</v>
@@ -15485,7 +15449,7 @@
         <v>1</v>
       </c>
       <c r="K87" s="23" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="M87">
         <v>87</v>
@@ -15505,7 +15469,7 @@
         <v>1</v>
       </c>
       <c r="K88" s="23" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="M88">
         <v>88</v>
@@ -15525,7 +15489,7 @@
         <v>1</v>
       </c>
       <c r="K89" s="23" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="M89">
         <v>89</v>
@@ -15545,7 +15509,7 @@
         <v>1</v>
       </c>
       <c r="K90" s="23" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="M90">
         <v>90</v>
@@ -15565,7 +15529,7 @@
         <v>1</v>
       </c>
       <c r="K91" s="23" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="M91">
         <v>91</v>
@@ -15585,7 +15549,7 @@
         <v>1</v>
       </c>
       <c r="K92" s="23" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="M92">
         <v>92</v>
@@ -15753,7 +15717,7 @@
     </row>
     <row r="102" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C102">
         <v>1</v>
@@ -15787,7 +15751,7 @@
     </row>
     <row r="104" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C104">
         <v>1</v>
@@ -15804,7 +15768,7 @@
     </row>
     <row r="105" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C105">
         <v>1</v>
@@ -15957,7 +15921,7 @@
     </row>
     <row r="114" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -15974,7 +15938,7 @@
     </row>
     <row r="115" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -15991,7 +15955,7 @@
     </row>
     <row r="116" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -16008,7 +15972,7 @@
     </row>
     <row r="117" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C117">
         <v>0</v>
@@ -16025,7 +15989,7 @@
     </row>
     <row r="118" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C118">
         <v>0</v>
@@ -16042,7 +16006,7 @@
     </row>
     <row r="119" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C119">
         <v>0</v>
@@ -16059,7 +16023,7 @@
     </row>
     <row r="120" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C120">
         <v>0</v>
@@ -16076,7 +16040,7 @@
     </row>
     <row r="121" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -16093,7 +16057,7 @@
     </row>
     <row r="122" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C122">
         <v>0</v>
@@ -16110,7 +16074,7 @@
     </row>
     <row r="123" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C123">
         <v>0</v>
@@ -16127,7 +16091,7 @@
     </row>
     <row r="124" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C124">
         <v>0</v>
@@ -16135,7 +16099,7 @@
     </row>
     <row r="125" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C125">
         <v>0</v>
@@ -16143,7 +16107,7 @@
     </row>
     <row r="126" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C126">
         <v>0</v>
@@ -16151,7 +16115,7 @@
     </row>
     <row r="127" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C127">
         <v>0</v>
@@ -16159,7 +16123,7 @@
     </row>
     <row r="128" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C128">
         <v>0</v>
@@ -16167,7 +16131,7 @@
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C129">
         <v>0</v>
@@ -16175,7 +16139,7 @@
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C130">
         <v>0</v>
@@ -16183,7 +16147,7 @@
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C131">
         <v>0</v>
@@ -16191,7 +16155,7 @@
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -16199,7 +16163,7 @@
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -16207,7 +16171,7 @@
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -16215,7 +16179,7 @@
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -16223,7 +16187,7 @@
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -16231,7 +16195,7 @@
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -16239,7 +16203,7 @@
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -16247,7 +16211,7 @@
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C139">
         <v>0</v>
@@ -16255,7 +16219,7 @@
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C140">
         <v>0</v>
@@ -16263,7 +16227,7 @@
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C141">
         <v>0</v>
@@ -16271,7 +16235,7 @@
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C142">
         <v>0</v>
@@ -16279,7 +16243,7 @@
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C143">
         <v>0</v>
@@ -16287,7 +16251,7 @@
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C144">
         <v>0</v>
@@ -16295,7 +16259,7 @@
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C145">
         <v>0</v>
@@ -16303,7 +16267,7 @@
     </row>
     <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C146">
         <v>0</v>
@@ -16311,7 +16275,7 @@
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C147">
         <v>0</v>
@@ -16319,7 +16283,7 @@
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C148">
         <v>0</v>
@@ -16327,7 +16291,7 @@
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C149">
         <v>0</v>
@@ -16335,7 +16299,7 @@
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C150">
         <v>0</v>
@@ -16343,7 +16307,7 @@
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C151">
         <v>0</v>
@@ -16351,7 +16315,7 @@
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C152">
         <v>0</v>
@@ -16359,7 +16323,7 @@
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C153">
         <v>1</v>

</xml_diff>